<commit_message>
final plotting and final docs
</commit_message>
<xml_diff>
--- a/Documents/Stats.xlsx
+++ b/Documents/Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\source\repos\ShadNick\MLPraktikum\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D544089-30CB-4A77-BBA0-DE1CEABA6707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A807F23-8645-48C7-8409-CD23EE5BD021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{C50481C0-3E7F-4500-ADDA-BEE2E952B991}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="92">
   <si>
     <t>Model</t>
   </si>
@@ -316,6 +316,24 @@
   </si>
   <si>
     <t>andere algorithm</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Multi</t>
+  </si>
+  <si>
+    <t>KNN Cancer</t>
+  </si>
+  <si>
+    <t>Regression</t>
+  </si>
+  <si>
+    <t>Peak Diff Outliner</t>
   </si>
 </sst>
 </file>
@@ -339,7 +357,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -457,11 +475,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -527,6 +554,10 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -872,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18C823A-5B43-45CA-919F-52C1C837F365}">
   <dimension ref="A1:AE173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T91" sqref="T91"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -884,6 +915,8 @@
     <col min="7" max="7" width="15.54296875" style="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.90625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="25.1796875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.54296875" bestFit="1" customWidth="1"/>
@@ -904,16 +937,16 @@
       <c r="I1" s="14"/>
       <c r="J1" s="6"/>
       <c r="R1" s="7"/>
-      <c r="S1" s="31" t="s">
+      <c r="S1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="31" t="s">
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="33"/>
+      <c r="X1" s="35"/>
       <c r="Z1" s="14"/>
       <c r="AA1" s="6"/>
     </row>
@@ -976,23 +1009,23 @@
         <v>1</v>
       </c>
       <c r="B3" s="10">
-        <v>5.79</v>
+        <v>5.77</v>
       </c>
       <c r="C3" s="10">
-        <v>5.92</v>
+        <v>5.94</v>
       </c>
       <c r="D3" s="10">
         <v>6.06</v>
       </c>
       <c r="E3" s="12">
-        <v>5.91</v>
+        <v>5.89</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="12"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10">
         <f>AVERAGE(B3:E3)</f>
-        <v>5.92</v>
+        <v>5.915</v>
       </c>
       <c r="J3" s="12"/>
       <c r="O3" s="8"/>
@@ -1025,13 +1058,13 @@
         <v>5</v>
       </c>
       <c r="B4" s="10">
+        <v>5.78</v>
+      </c>
+      <c r="C4" s="10">
         <v>6.12</v>
       </c>
-      <c r="C4" s="10">
+      <c r="D4" s="10">
         <v>5.78</v>
-      </c>
-      <c r="D4" s="10">
-        <v>5.97</v>
       </c>
       <c r="E4" s="12">
         <v>5.86</v>
@@ -1041,7 +1074,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10">
         <f>AVERAGE(B4:E4)</f>
-        <v>5.9325000000000001</v>
+        <v>5.8849999999999998</v>
       </c>
       <c r="J4" s="12"/>
       <c r="O4" s="8"/>
@@ -1093,6 +1126,15 @@
         <v>5.8649999999999993</v>
       </c>
       <c r="J5" s="12"/>
+      <c r="L5" t="s">
+        <v>54</v>
+      </c>
+      <c r="M5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" t="s">
+        <v>56</v>
+      </c>
       <c r="O5" s="8"/>
       <c r="R5" s="6" t="s">
         <v>6</v>
@@ -1123,25 +1165,37 @@
         <v>7</v>
       </c>
       <c r="B6" s="10">
-        <v>5.72</v>
+        <v>5.77</v>
       </c>
       <c r="C6" s="10">
-        <v>5.81</v>
+        <v>5.29</v>
       </c>
       <c r="D6" s="10">
-        <v>5.94</v>
+        <v>5.91</v>
       </c>
       <c r="E6" s="12">
-        <v>5.55</v>
+        <v>5.99</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="12"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10">
         <f>AVERAGE(B6:E6)</f>
-        <v>5.7549999999999999</v>
+        <v>5.74</v>
       </c>
       <c r="J6" s="12"/>
+      <c r="L6" s="1" cm="1">
+        <f t="array" ref="L6:L17">_xlfn._xlws.SORT(_xlfn.UNIQUE(J21:J51), ,-1)</f>
+        <v>100</v>
+      </c>
+      <c r="M6" s="10">
+        <f>COUNTIF($J$21:$J$51,L6)</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="24">
+        <f>M6/$M$18</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
       <c r="O6" s="8"/>
       <c r="R6" s="6" t="s">
         <v>7</v>
@@ -1172,25 +1226,36 @@
         <v>8</v>
       </c>
       <c r="B7" s="11">
-        <v>5.73</v>
+        <v>5.72</v>
       </c>
       <c r="C7" s="11">
-        <v>5.77</v>
+        <v>5.42</v>
       </c>
       <c r="D7" s="11">
-        <v>5.96</v>
+        <v>5.85</v>
       </c>
       <c r="E7" s="13">
-        <v>5.29</v>
+        <v>5.56</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="13"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11">
         <f>AVERAGE(B7:E7)</f>
-        <v>5.6875</v>
+        <v>5.6375000000000002</v>
       </c>
       <c r="J7" s="13"/>
+      <c r="L7" s="1">
+        <v>99</v>
+      </c>
+      <c r="M7" s="10">
+        <f t="shared" ref="M7:M17" si="0">COUNTIF($J$21:$J$51,L7)</f>
+        <v>4</v>
+      </c>
+      <c r="N7" s="24">
+        <f t="shared" ref="N7:N17" si="1">M7/$M$18</f>
+        <v>0.13333333333333333</v>
+      </c>
       <c r="O7" s="8"/>
       <c r="R7" s="7" t="s">
         <v>8</v>
@@ -1225,17 +1290,28 @@
       <c r="D8" s="10"/>
       <c r="E8" s="12"/>
       <c r="F8" s="20">
-        <v>5.62</v>
+        <v>5.78</v>
       </c>
       <c r="G8" s="12">
-        <v>6.24</v>
+        <v>5.81</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10">
         <f>AVERAGE(F8:G8)</f>
-        <v>5.93</v>
+        <v>5.7949999999999999</v>
       </c>
       <c r="J8" s="12"/>
+      <c r="L8" s="1">
+        <v>98</v>
+      </c>
+      <c r="M8" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N8" s="24">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
       <c r="O8" s="9"/>
       <c r="R8" s="6" t="s">
         <v>31</v>
@@ -1273,10 +1349,21 @@
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10">
-        <f t="shared" ref="I9:I12" si="0">AVERAGE(F9:G9)</f>
+        <f t="shared" ref="I9:I12" si="2">AVERAGE(F9:G9)</f>
         <v>6</v>
       </c>
       <c r="J9" s="12"/>
+      <c r="L9" s="1">
+        <v>97</v>
+      </c>
+      <c r="M9" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N9" s="24">
+        <f t="shared" si="1"/>
+        <v>0.13333333333333333</v>
+      </c>
       <c r="O9" s="9"/>
       <c r="R9" s="6" t="s">
         <v>32</v>
@@ -1293,7 +1380,7 @@
       </c>
       <c r="Y9" s="10"/>
       <c r="Z9" s="10">
-        <f t="shared" ref="Z9" si="1">AVERAGE(W9:X9)</f>
+        <f t="shared" ref="Z9" si="3">AVERAGE(W9:X9)</f>
         <v>7.335</v>
       </c>
       <c r="AA9" s="12"/>
@@ -1318,6 +1405,17 @@
         <v>5.875</v>
       </c>
       <c r="J10" s="12"/>
+      <c r="L10" s="1">
+        <v>96</v>
+      </c>
+      <c r="M10" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="N10" s="24">
+        <f t="shared" si="1"/>
+        <v>0.13333333333333333</v>
+      </c>
       <c r="O10" s="9"/>
       <c r="R10" s="6" t="s">
         <v>33</v>
@@ -1355,10 +1453,21 @@
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10">
+        <f t="shared" si="2"/>
+        <v>6.17</v>
+      </c>
+      <c r="J11" s="12"/>
+      <c r="L11" s="1">
+        <v>95</v>
+      </c>
+      <c r="M11" s="10">
         <f t="shared" si="0"/>
-        <v>6.17</v>
-      </c>
-      <c r="J11" s="12"/>
+        <v>9</v>
+      </c>
+      <c r="N11" s="24">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
       <c r="R11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1374,7 +1483,7 @@
       </c>
       <c r="Y11" s="10"/>
       <c r="Z11" s="10">
-        <f t="shared" ref="Z11:Z12" si="2">AVERAGE(W11:X11)</f>
+        <f t="shared" ref="Z11:Z12" si="4">AVERAGE(W11:X11)</f>
         <v>7.32</v>
       </c>
       <c r="AA11" s="12"/>
@@ -1395,10 +1504,21 @@
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11">
+        <f t="shared" si="2"/>
+        <v>5.9649999999999999</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="L12" s="1">
+        <v>94</v>
+      </c>
+      <c r="M12" s="10">
         <f t="shared" si="0"/>
-        <v>5.9649999999999999</v>
-      </c>
-      <c r="J12" s="13"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="24">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
       <c r="R12" s="7" t="s">
         <v>35</v>
       </c>
@@ -1414,7 +1534,7 @@
       </c>
       <c r="Y12" s="11"/>
       <c r="Z12" s="11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7.2200000000000006</v>
       </c>
       <c r="AA12" s="13"/>
@@ -1430,6 +1550,17 @@
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="12"/>
+      <c r="L13" s="1">
+        <v>93</v>
+      </c>
+      <c r="M13" s="10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="N13" s="24">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
       <c r="R13" s="6"/>
       <c r="S13" s="10"/>
       <c r="T13" s="10"/>
@@ -1447,34 +1578,45 @@
       </c>
       <c r="B14" s="10">
         <f>AVERAGE(B3:B7)</f>
-        <v>5.9</v>
+        <v>5.8360000000000003</v>
       </c>
       <c r="C14" s="10">
         <f>AVERAGE(C3:C7)</f>
-        <v>5.7859999999999996</v>
+        <v>5.6840000000000002</v>
       </c>
       <c r="D14" s="10">
         <f>AVERAGE(D3:D7)</f>
-        <v>6.0260000000000007</v>
+        <v>5.9599999999999991</v>
       </c>
       <c r="E14" s="12">
         <f>AVERAGE(E3:E7)</f>
-        <v>5.6159999999999997</v>
+        <v>5.7539999999999996</v>
       </c>
       <c r="F14" s="10">
         <f>AVERAGE(F8:F12)</f>
-        <v>5.8839999999999995</v>
+        <v>5.9160000000000004</v>
       </c>
       <c r="G14" s="12">
         <f>AVERAGE(G8:G12)</f>
-        <v>6.0920000000000005</v>
+        <v>6.0060000000000002</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10">
         <f>AVERAGE(B14:G14,I3:I12)</f>
-        <v>5.9002500000000007</v>
+        <v>5.8752187500000002</v>
       </c>
       <c r="J14" s="12"/>
+      <c r="L14" s="1">
+        <v>91</v>
+      </c>
+      <c r="M14" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N14" s="24">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
       <c r="R14" s="6" t="s">
         <v>49</v>
       </c>
@@ -1520,6 +1662,17 @@
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
       <c r="J15" s="13"/>
+      <c r="L15" s="1">
+        <v>90</v>
+      </c>
+      <c r="M15" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N15" s="24">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
       <c r="R15" s="7"/>
       <c r="S15" s="11"/>
       <c r="T15" s="11"/>
@@ -1542,6 +1695,17 @@
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="15"/>
+      <c r="L16" s="1">
+        <v>88</v>
+      </c>
+      <c r="M16" s="10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N16" s="24">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
       <c r="R16" s="6"/>
       <c r="S16" s="14"/>
       <c r="T16" s="14"/>
@@ -1563,6 +1727,24 @@
       <c r="G17" s="22"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N17" s="24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="M18" s="14">
+        <f>SUM(M6:M17)</f>
+        <v>30</v>
+      </c>
+      <c r="N18" s="26"/>
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -1601,6 +1783,13 @@
       <c r="J20" s="11" t="s">
         <v>51</v>
       </c>
+      <c r="L20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N20" s="1"/>
       <c r="P20" s="25"/>
       <c r="S20" s="2">
         <v>4</v>
@@ -1635,32 +1824,39 @@
         <v>11</v>
       </c>
       <c r="B21" s="10">
-        <v>29.9</v>
+        <v>30.21</v>
       </c>
       <c r="C21" s="10">
-        <v>20.62</v>
+        <v>20.83</v>
       </c>
       <c r="D21" s="10">
-        <v>19.59</v>
+        <v>20.83</v>
       </c>
       <c r="E21" s="10">
-        <v>12.37</v>
+        <v>10.42</v>
       </c>
       <c r="F21" s="10">
-        <v>6.19</v>
+        <v>6.25</v>
       </c>
       <c r="G21" s="10">
-        <v>10.31</v>
+        <v>10.42</v>
       </c>
       <c r="H21" s="10">
-        <v>1.03</v>
+        <v>1.04</v>
       </c>
       <c r="I21" s="10">
-        <v>0.60375000000000001</v>
+        <v>0.59636</v>
       </c>
       <c r="J21" s="10">
-        <v>95</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M21" s="10">
+        <v>1.9</v>
+      </c>
+      <c r="N21" s="1"/>
       <c r="P21" s="25"/>
       <c r="R21" t="s">
         <v>11</v>
@@ -1698,10 +1894,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="10">
-        <v>33.340000000000003</v>
+        <v>33.33</v>
       </c>
       <c r="C22" s="10">
-        <v>15.15</v>
+        <v>16.16</v>
       </c>
       <c r="D22" s="10">
         <v>14.14</v>
@@ -1710,20 +1906,27 @@
         <v>13.13</v>
       </c>
       <c r="F22" s="10">
-        <v>10.1</v>
+        <v>9.09</v>
       </c>
       <c r="G22" s="10">
-        <v>10.1</v>
+        <v>11.11</v>
       </c>
       <c r="H22" s="10">
         <v>3.03</v>
       </c>
       <c r="I22" s="10">
-        <v>1.63245</v>
+        <v>1.6642999999999999</v>
       </c>
       <c r="J22" s="10">
         <v>95</v>
       </c>
+      <c r="L22" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M22" s="10">
+        <v>10.3</v>
+      </c>
+      <c r="N22" s="1"/>
       <c r="P22" s="25"/>
       <c r="R22" t="s">
         <v>12</v>
@@ -1787,6 +1990,13 @@
       <c r="J23" s="10">
         <v>99</v>
       </c>
+      <c r="L23" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M23" s="10">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N23" s="1"/>
       <c r="P23" s="25"/>
       <c r="R23" t="s">
         <v>13</v>
@@ -1827,13 +2037,13 @@
         <v>27.27</v>
       </c>
       <c r="C24" s="10">
-        <v>17.71</v>
+        <v>18.18</v>
       </c>
       <c r="D24" s="10">
         <v>21.21</v>
       </c>
       <c r="E24" s="10">
-        <v>19.190000000000001</v>
+        <v>18.18</v>
       </c>
       <c r="F24" s="10">
         <v>6.06</v>
@@ -1845,11 +2055,18 @@
         <v>4.04</v>
       </c>
       <c r="I24" s="10">
-        <v>1.2533399999999999</v>
+        <v>1.2583299999999999</v>
       </c>
       <c r="J24" s="10">
         <v>98</v>
       </c>
+      <c r="L24" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M24" s="10">
+        <v>4.7</v>
+      </c>
+      <c r="N24" s="1"/>
       <c r="P24" s="25"/>
       <c r="R24" t="s">
         <v>14</v>
@@ -1887,32 +2104,39 @@
         <v>15</v>
       </c>
       <c r="B25" s="10">
-        <v>23.96</v>
+        <v>25.26</v>
       </c>
       <c r="C25" s="10">
-        <v>21.88</v>
+        <v>23.16</v>
       </c>
       <c r="D25" s="10">
-        <v>19.79</v>
+        <v>24.11</v>
       </c>
       <c r="E25" s="10">
-        <v>11.46</v>
+        <v>11.58</v>
       </c>
       <c r="F25" s="10">
-        <v>6.25</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="G25" s="10">
-        <v>8.33</v>
+        <v>4.21</v>
       </c>
       <c r="H25" s="10">
-        <v>8.33</v>
+        <v>2.11</v>
       </c>
       <c r="I25" s="10">
-        <v>0.77769999999999995</v>
+        <v>0.89058000000000004</v>
       </c>
       <c r="J25" s="10">
         <v>95</v>
       </c>
+      <c r="L25" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M25" s="10">
+        <v>3.4</v>
+      </c>
+      <c r="N25" s="1"/>
       <c r="P25" s="25"/>
       <c r="R25" t="s">
         <v>15</v>
@@ -1950,32 +2174,39 @@
         <v>16</v>
       </c>
       <c r="B26" s="10">
-        <v>33.33</v>
+        <v>28</v>
       </c>
       <c r="C26" s="10">
-        <v>14.14</v>
+        <v>11</v>
       </c>
       <c r="D26" s="10">
-        <v>22.22</v>
+        <v>23</v>
       </c>
       <c r="E26" s="10">
-        <v>13.13</v>
+        <v>11</v>
       </c>
       <c r="F26" s="10">
-        <v>9.09</v>
+        <v>16</v>
       </c>
       <c r="G26" s="10">
-        <v>5.05</v>
+        <v>8</v>
       </c>
       <c r="H26" s="10">
-        <v>3.03</v>
+        <v>3</v>
       </c>
       <c r="I26" s="10">
-        <v>1.5426200000000001</v>
+        <v>1.50482</v>
       </c>
       <c r="J26" s="10">
-        <v>98</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M26" s="10">
+        <v>7.2</v>
+      </c>
+      <c r="N26" s="1"/>
       <c r="P26" s="25"/>
       <c r="R26" t="s">
         <v>16</v>
@@ -2013,32 +2244,39 @@
         <v>17</v>
       </c>
       <c r="B27" s="10">
-        <v>30.53</v>
+        <v>25.25</v>
       </c>
       <c r="C27" s="10">
-        <v>20</v>
+        <v>25.25</v>
       </c>
       <c r="D27" s="10">
-        <v>11.58</v>
+        <v>21.21</v>
       </c>
       <c r="E27" s="10">
-        <v>12.63</v>
+        <v>13.13</v>
       </c>
       <c r="F27" s="10">
-        <v>15.79</v>
+        <v>8.08</v>
       </c>
       <c r="G27" s="10">
-        <v>4.21</v>
+        <v>4.04</v>
       </c>
       <c r="H27" s="10">
-        <v>5.26</v>
+        <v>3.03</v>
       </c>
       <c r="I27" s="10">
-        <v>0.61599999999999999</v>
+        <v>0.64427000000000001</v>
       </c>
       <c r="J27" s="10">
         <v>99</v>
       </c>
+      <c r="L27" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M27" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N27" s="1"/>
       <c r="P27" s="25"/>
       <c r="R27" t="s">
         <v>17</v>
@@ -2076,32 +2314,39 @@
         <v>18</v>
       </c>
       <c r="B28" s="10">
-        <v>33.33</v>
+        <v>30.93</v>
       </c>
       <c r="C28" s="10">
-        <v>15.62</v>
+        <v>15.46</v>
       </c>
       <c r="D28" s="10">
-        <v>17.71</v>
+        <v>18.559999999999999</v>
       </c>
       <c r="E28" s="10">
-        <v>11.46</v>
+        <v>18.559999999999999</v>
       </c>
       <c r="F28" s="10">
-        <v>12.5</v>
+        <v>9.2799999999999994</v>
       </c>
       <c r="G28" s="10">
-        <v>5.21</v>
+        <v>3.09</v>
       </c>
       <c r="H28" s="10">
-        <v>4.17</v>
+        <v>4.12</v>
       </c>
       <c r="I28" s="10">
-        <v>1.68625</v>
+        <v>1.6086</v>
       </c>
       <c r="J28" s="10">
-        <v>95</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="L28" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M28" s="10">
+        <v>8</v>
+      </c>
+      <c r="N28" s="1"/>
       <c r="P28" s="25"/>
       <c r="R28" t="s">
         <v>18</v>
@@ -2165,6 +2410,13 @@
       <c r="J29" s="10">
         <v>93</v>
       </c>
+      <c r="L29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M29" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="N29" s="1"/>
       <c r="P29" s="25"/>
       <c r="R29" t="s">
         <v>19</v>
@@ -2228,6 +2480,13 @@
       <c r="J30" s="10">
         <v>99</v>
       </c>
+      <c r="L30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M30" s="10">
+        <v>5</v>
+      </c>
+      <c r="N30" s="1"/>
       <c r="P30" s="25"/>
       <c r="R30" t="s">
         <v>20</v>
@@ -2291,6 +2550,13 @@
       <c r="J31" s="10">
         <v>96</v>
       </c>
+      <c r="L31" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M31" s="10">
+        <v>3.3</v>
+      </c>
+      <c r="N31" s="1"/>
       <c r="P31" s="25"/>
       <c r="R31" t="s">
         <v>21</v>
@@ -2354,6 +2620,13 @@
       <c r="J32" s="10">
         <v>96</v>
       </c>
+      <c r="L32" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M32" s="10">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N32" s="1"/>
       <c r="P32" s="25"/>
       <c r="R32" t="s">
         <v>22</v>
@@ -2388,35 +2661,42 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="B33" s="10">
-        <v>29.9</v>
+        <v>29.79</v>
       </c>
       <c r="C33" s="10">
-        <v>18.559999999999999</v>
+        <v>19.149999999999999</v>
       </c>
       <c r="D33" s="10">
-        <v>26.8</v>
+        <v>22.34</v>
       </c>
       <c r="E33" s="10">
-        <v>8.25</v>
+        <v>11.7</v>
       </c>
       <c r="F33" s="10">
-        <v>9.2799999999999994</v>
+        <v>9.57</v>
       </c>
       <c r="G33" s="10">
-        <v>5.15</v>
+        <v>5.32</v>
       </c>
       <c r="H33" s="10">
-        <v>2.06</v>
+        <v>2.13</v>
       </c>
       <c r="I33" s="10">
-        <v>0.65769</v>
+        <v>0.78122999999999998</v>
       </c>
       <c r="J33" s="10">
         <v>93</v>
       </c>
+      <c r="L33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M33" s="10">
+        <v>2.7</v>
+      </c>
+      <c r="N33" s="1"/>
       <c r="P33" s="25"/>
       <c r="R33" t="s">
         <v>23</v>
@@ -2454,32 +2734,39 @@
         <v>24</v>
       </c>
       <c r="B34" s="10">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C34" s="10">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D34" s="10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E34" s="10">
         <v>14</v>
       </c>
       <c r="F34" s="10">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G34" s="10">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H34" s="10">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I34" s="10">
-        <v>1.53356</v>
+        <v>1.43398</v>
       </c>
       <c r="J34" s="10">
-        <v>96</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M34" s="10">
+        <v>5.3</v>
+      </c>
+      <c r="N34" s="1"/>
       <c r="P34" s="25"/>
       <c r="R34" t="s">
         <v>24</v>
@@ -2517,32 +2804,39 @@
         <v>25</v>
       </c>
       <c r="B35" s="10">
-        <v>22.68</v>
+        <v>25</v>
       </c>
       <c r="C35" s="10">
-        <v>24.74</v>
+        <v>22.92</v>
       </c>
       <c r="D35" s="10">
-        <v>20.62</v>
+        <v>17.71</v>
       </c>
       <c r="E35" s="10">
-        <v>13.4</v>
+        <v>15.62</v>
       </c>
       <c r="F35" s="10">
-        <v>8.25</v>
+        <v>10.42</v>
       </c>
       <c r="G35" s="10">
-        <v>7.22</v>
+        <v>6.25</v>
       </c>
       <c r="H35" s="10">
-        <v>3.09</v>
+        <v>2</v>
       </c>
       <c r="I35" s="10">
-        <v>0.24301</v>
+        <v>0.17602999999999999</v>
       </c>
       <c r="J35" s="10">
-        <v>99</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M35" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="N35" s="1"/>
       <c r="P35" s="25"/>
       <c r="R35" t="s">
         <v>25</v>
@@ -2589,32 +2883,39 @@
         <v>26</v>
       </c>
       <c r="B36" s="10">
-        <v>32.65</v>
+        <v>22.45</v>
       </c>
       <c r="C36" s="10">
+        <v>20.41</v>
+      </c>
+      <c r="D36" s="10">
+        <v>23.47</v>
+      </c>
+      <c r="E36" s="10">
+        <v>14.29</v>
+      </c>
+      <c r="F36" s="10">
         <v>10.199999999999999</v>
       </c>
-      <c r="D36" s="10">
-        <v>32.65</v>
-      </c>
-      <c r="E36" s="10">
-        <v>18.37</v>
-      </c>
-      <c r="F36" s="10">
-        <v>6.12</v>
-      </c>
       <c r="G36" s="10">
-        <v>0</v>
+        <v>7.14</v>
       </c>
       <c r="H36" s="10">
-        <v>0</v>
+        <v>2.04</v>
       </c>
       <c r="I36" s="10">
-        <v>1.18191</v>
+        <v>3.1112099999999998</v>
       </c>
       <c r="J36" s="10">
-        <v>93</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M36" s="10">
+        <v>15.3</v>
+      </c>
+      <c r="N36" s="1"/>
       <c r="P36" s="25"/>
       <c r="R36" t="s">
         <v>26</v>
@@ -2664,41 +2965,39 @@
         <v>27</v>
       </c>
       <c r="B37" s="10">
-        <v>28.57</v>
+        <v>28.12</v>
       </c>
       <c r="C37" s="10">
-        <v>22.45</v>
+        <v>23.96</v>
       </c>
       <c r="D37" s="10">
-        <v>20.41</v>
+        <v>17.71</v>
       </c>
       <c r="E37" s="10">
-        <v>15.31</v>
+        <v>17.71</v>
       </c>
       <c r="F37" s="10">
-        <v>6.12</v>
+        <v>5.21</v>
       </c>
       <c r="G37" s="10">
-        <v>3.06</v>
+        <v>5.21</v>
       </c>
       <c r="H37" s="10">
-        <v>4.08</v>
+        <v>2.08</v>
       </c>
       <c r="I37" s="10">
-        <v>0.46178000000000002</v>
+        <v>0.73428000000000004</v>
       </c>
       <c r="J37" s="10">
-        <v>94</v>
-      </c>
-      <c r="L37" t="s">
-        <v>54</v>
-      </c>
-      <c r="M37" t="s">
-        <v>55</v>
-      </c>
-      <c r="N37" t="s">
-        <v>56</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="L37" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="M37" s="10">
+        <v>2.6</v>
+      </c>
+      <c r="N37" s="1"/>
       <c r="P37" s="25"/>
       <c r="R37" t="s">
         <v>27</v>
@@ -2738,7 +3037,7 @@
         <v>1</v>
       </c>
       <c r="AE37" s="24">
-        <f t="shared" ref="AE37:AE51" si="3">AD37/$AD$54</f>
+        <f t="shared" ref="AE37:AE51" si="5">AD37/$AD$54</f>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -2747,41 +3046,39 @@
         <v>28</v>
       </c>
       <c r="B38" s="10">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C38" s="10">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D38" s="10">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E38" s="10">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F38" s="10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G38" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H38" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I38" s="10">
-        <v>1.45756</v>
+        <v>1.4186300000000001</v>
       </c>
       <c r="J38" s="10">
-        <v>96</v>
-      </c>
-      <c r="L38" s="1">
-        <v>99</v>
-      </c>
-      <c r="M38" s="1">
-        <v>5</v>
-      </c>
-      <c r="N38" s="10">
-        <v>16.670000000000002</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M38" s="10">
+        <v>5.3</v>
+      </c>
+      <c r="N38" s="1"/>
       <c r="P38" s="25"/>
       <c r="R38" t="s">
         <v>28</v>
@@ -2821,7 +3118,7 @@
         <v>2</v>
       </c>
       <c r="AE38" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.8965517241379309E-2</v>
       </c>
     </row>
@@ -2830,41 +3127,39 @@
         <v>29</v>
       </c>
       <c r="B39" s="10">
-        <v>26.26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="10">
-        <v>17.170000000000002</v>
+        <v>20.83</v>
       </c>
       <c r="D39" s="10">
-        <v>21.21</v>
+        <v>23.96</v>
       </c>
       <c r="E39" s="10">
-        <v>13.13</v>
+        <v>12.5</v>
       </c>
       <c r="F39" s="10">
-        <v>16.16</v>
+        <v>11.46</v>
       </c>
       <c r="G39" s="10">
-        <v>4.04</v>
+        <v>4.17</v>
       </c>
       <c r="H39" s="10">
-        <v>2.02</v>
+        <v>2.08</v>
       </c>
       <c r="I39" s="10">
-        <v>0.26721</v>
+        <v>0.27718999999999999</v>
       </c>
       <c r="J39" s="10">
-        <v>99</v>
-      </c>
-      <c r="L39" s="1">
-        <v>98</v>
-      </c>
-      <c r="M39" s="1">
-        <v>3</v>
-      </c>
-      <c r="N39" s="10">
-        <v>10</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M39" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="N39" s="1"/>
       <c r="P39" s="25"/>
       <c r="R39" t="s">
         <v>29</v>
@@ -2904,7 +3199,7 @@
         <v>2</v>
       </c>
       <c r="AE39" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.8965517241379309E-2</v>
       </c>
     </row>
@@ -2913,41 +3208,39 @@
         <v>30</v>
       </c>
       <c r="B40" s="10">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C40" s="10">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D40" s="10">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E40" s="10">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="F40" s="10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G40" s="10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H40" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40" s="10">
-        <v>0.74690000000000001</v>
+        <v>1.39438</v>
       </c>
       <c r="J40" s="10">
-        <v>98</v>
-      </c>
-      <c r="L40" s="1">
-        <v>97</v>
-      </c>
-      <c r="M40" s="1">
-        <v>5</v>
-      </c>
-      <c r="N40" s="10">
-        <v>16.670000000000002</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="L40" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="M40" s="10">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N40" s="1"/>
       <c r="P40" s="25"/>
       <c r="R40" t="s">
         <v>30</v>
@@ -2987,7 +3280,7 @@
         <v>4</v>
       </c>
       <c r="AE40" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.13793103448275862</v>
       </c>
     </row>
@@ -3001,15 +3294,9 @@
       <c r="H41" s="10"/>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
-      <c r="L41" s="1">
-        <v>96</v>
-      </c>
-      <c r="M41" s="1">
-        <v>4</v>
-      </c>
-      <c r="N41" s="10">
-        <v>13.33</v>
-      </c>
+      <c r="L41" s="8"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="1"/>
       <c r="P41" s="25"/>
       <c r="S41" s="10"/>
       <c r="T41" s="10"/>
@@ -3028,7 +3315,7 @@
         <v>1</v>
       </c>
       <c r="AE41" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -3037,41 +3324,39 @@
         <v>39</v>
       </c>
       <c r="B42" s="10">
-        <v>31.18</v>
+        <v>32.29</v>
       </c>
       <c r="C42" s="10">
-        <v>22.58</v>
+        <v>20.83</v>
       </c>
       <c r="D42" s="10">
-        <v>19.350000000000001</v>
+        <v>15.62</v>
       </c>
       <c r="E42" s="10">
-        <v>13.98</v>
+        <v>11.46</v>
       </c>
       <c r="F42" s="10">
-        <v>7.53</v>
+        <v>9.3800000000000008</v>
       </c>
       <c r="G42" s="10">
-        <v>3.23</v>
+        <v>8.33</v>
       </c>
       <c r="H42" s="10">
-        <v>2.15</v>
+        <v>2.08</v>
       </c>
       <c r="I42" s="10">
-        <v>2.5718999999999999</v>
+        <v>2.83501</v>
       </c>
       <c r="J42" s="10">
-        <v>91</v>
-      </c>
-      <c r="L42" s="1">
-        <v>95</v>
-      </c>
-      <c r="M42" s="1">
-        <v>7</v>
-      </c>
-      <c r="N42" s="10">
-        <v>23.33</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="L42" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M42" s="10">
+        <v>12</v>
+      </c>
+      <c r="N42" s="1"/>
       <c r="P42" s="25"/>
       <c r="R42" t="s">
         <v>39</v>
@@ -3111,7 +3396,7 @@
         <v>1</v>
       </c>
       <c r="AE42" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -3120,41 +3405,39 @@
         <v>40</v>
       </c>
       <c r="B43" s="10">
-        <v>23.71</v>
+        <v>29.47</v>
       </c>
       <c r="C43" s="10">
-        <v>15.46</v>
+        <v>16.84</v>
       </c>
       <c r="D43" s="10">
-        <v>21.65</v>
+        <v>25.26</v>
       </c>
       <c r="E43" s="10">
-        <v>12.37</v>
+        <v>10.53</v>
       </c>
       <c r="F43" s="10">
-        <v>13.4</v>
+        <v>9.4700000000000006</v>
       </c>
       <c r="G43" s="10">
-        <v>6.19</v>
+        <v>6.32</v>
       </c>
       <c r="H43" s="10">
-        <v>7.22</v>
+        <v>2.11</v>
       </c>
       <c r="I43" s="10">
-        <v>0.61778</v>
+        <v>0.61273999999999995</v>
       </c>
       <c r="J43" s="10">
-        <v>97</v>
-      </c>
-      <c r="L43" s="1">
-        <v>94</v>
-      </c>
-      <c r="M43" s="1">
-        <v>1</v>
-      </c>
-      <c r="N43" s="10">
-        <v>3.33</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="L43" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M43" s="10">
+        <v>2.8</v>
+      </c>
+      <c r="N43" s="1"/>
       <c r="P43" s="25"/>
       <c r="R43" t="s">
         <v>40</v>
@@ -3194,7 +3477,7 @@
         <v>1</v>
       </c>
       <c r="AE43" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -3229,15 +3512,13 @@
       <c r="J44" s="10">
         <v>97</v>
       </c>
-      <c r="L44" s="1">
-        <v>93</v>
-      </c>
-      <c r="M44" s="1">
-        <v>3</v>
-      </c>
-      <c r="N44" s="10">
-        <v>10</v>
-      </c>
+      <c r="L44" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M44" s="10">
+        <v>11.5</v>
+      </c>
+      <c r="N44" s="1"/>
       <c r="P44" s="25"/>
       <c r="R44" t="s">
         <v>41</v>
@@ -3277,7 +3558,7 @@
         <v>1</v>
       </c>
       <c r="AE44" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -3312,15 +3593,13 @@
       <c r="J45" s="10">
         <v>97</v>
       </c>
-      <c r="L45" s="1">
-        <v>91</v>
-      </c>
-      <c r="M45" s="1">
-        <v>1</v>
-      </c>
-      <c r="N45" s="10">
-        <v>3.33</v>
-      </c>
+      <c r="L45" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M45" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="N45" s="1"/>
       <c r="P45" s="25"/>
       <c r="R45" t="s">
         <v>42</v>
@@ -3360,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="AE45" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -3395,15 +3674,13 @@
       <c r="J46" s="10">
         <v>90</v>
       </c>
-      <c r="L46" s="1">
+      <c r="L46" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="M46" s="1">
-        <v>1</v>
-      </c>
-      <c r="N46" s="10">
-        <v>3.33</v>
-      </c>
+      <c r="M46" s="10">
+        <v>10.5</v>
+      </c>
+      <c r="N46" s="1"/>
       <c r="P46" s="25"/>
       <c r="R46" t="s">
         <v>43</v>
@@ -3443,7 +3720,7 @@
         <v>1</v>
       </c>
       <c r="AE46" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -3478,7 +3755,13 @@
       <c r="J47" s="10">
         <v>97</v>
       </c>
-      <c r="N47" s="14"/>
+      <c r="L47" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M47" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="N47" s="10"/>
       <c r="P47" s="25"/>
       <c r="R47" t="s">
         <v>44</v>
@@ -3518,7 +3801,7 @@
         <v>1</v>
       </c>
       <c r="AE47" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -3553,6 +3836,13 @@
       <c r="J48" s="10">
         <v>97</v>
       </c>
+      <c r="L48" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M48" s="10">
+        <v>9.1</v>
+      </c>
+      <c r="N48" s="1"/>
       <c r="P48" s="25"/>
       <c r="R48" t="s">
         <v>45</v>
@@ -3592,7 +3882,7 @@
         <v>1</v>
       </c>
       <c r="AE48" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -3627,7 +3917,13 @@
       <c r="J49" s="10">
         <v>95</v>
       </c>
-      <c r="N49" s="14"/>
+      <c r="L49" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M49" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N49" s="10"/>
       <c r="P49" s="25"/>
       <c r="R49" t="s">
         <v>46</v>
@@ -3667,7 +3963,7 @@
         <v>4</v>
       </c>
       <c r="AE49" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.13793103448275862</v>
       </c>
     </row>
@@ -3702,6 +3998,13 @@
       <c r="J50" s="10">
         <v>95</v>
       </c>
+      <c r="L50" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M50" s="10">
+        <v>12.4</v>
+      </c>
+      <c r="N50" s="1"/>
       <c r="P50" s="25"/>
       <c r="R50" t="s">
         <v>47</v>
@@ -3741,7 +4044,7 @@
         <v>1</v>
       </c>
       <c r="AE50" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
@@ -3776,6 +4079,13 @@
       <c r="J51" s="10">
         <v>95</v>
       </c>
+      <c r="L51" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M51" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N51" s="1"/>
       <c r="P51" s="25"/>
       <c r="R51" t="s">
         <v>48</v>
@@ -3815,11 +4125,12 @@
         <v>1</v>
       </c>
       <c r="AE51" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>3.4482758620689655E-2</v>
       </c>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="L52" s="31"/>
       <c r="P52" s="25"/>
       <c r="S52" s="10"/>
       <c r="T52" s="10"/>
@@ -3848,36 +4159,36 @@
       </c>
       <c r="B53" s="10">
         <f>AVERAGE(B21:B40,B42:B51)</f>
-        <v>28.542666666666658</v>
+        <v>28.601333333333329</v>
       </c>
       <c r="C53" s="10">
-        <f t="shared" ref="C53:H53" si="4">AVERAGE(C21:C40,C42:C51)</f>
-        <v>17.534333333333333</v>
+        <f t="shared" ref="C53:G53" si="6">AVERAGE(C21:C40,C42:C51)</f>
+        <v>18.22433333333333</v>
       </c>
       <c r="D53" s="10">
-        <f t="shared" si="4"/>
-        <v>21.588999999999995</v>
+        <f t="shared" si="6"/>
+        <v>21.295666666666659</v>
       </c>
       <c r="E53" s="10">
-        <f t="shared" si="4"/>
-        <v>13.65433333333333</v>
+        <f t="shared" si="6"/>
+        <v>13.675333333333326</v>
       </c>
       <c r="F53" s="10">
-        <f t="shared" si="4"/>
-        <v>10.096000000000002</v>
+        <f t="shared" si="6"/>
+        <v>9.8993333333333347</v>
       </c>
       <c r="G53" s="10">
-        <f t="shared" si="4"/>
-        <v>5.0390000000000015</v>
+        <f t="shared" si="6"/>
+        <v>5.389333333333334</v>
       </c>
       <c r="H53" s="10">
-        <f t="shared" si="4"/>
-        <v>3.5943333333333332</v>
+        <f>AVERAGE(H21:H40,H42:H51)</f>
+        <v>2.9070000000000005</v>
       </c>
       <c r="I53" s="1"/>
       <c r="J53" s="14">
         <f>SUM(J21:J51)</f>
-        <v>2877</v>
+        <v>2863</v>
       </c>
       <c r="K53" s="14"/>
       <c r="P53" s="25"/>
@@ -3893,23 +4204,23 @@
         <v>20.185999999999996</v>
       </c>
       <c r="U53" s="10">
-        <f t="shared" ref="U53:Y53" si="5">AVERAGE(U21:U40,U42:U51)</f>
+        <f t="shared" ref="U53:Y53" si="7">AVERAGE(U21:U40,U42:U51)</f>
         <v>14.260333333333332</v>
       </c>
       <c r="V53" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>20.50866666666667</v>
       </c>
       <c r="W53" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>19.254999999999999</v>
       </c>
       <c r="X53" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>15.796999999999997</v>
       </c>
       <c r="Y53" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>10.323333333333334</v>
       </c>
       <c r="Z53" s="10"/>
@@ -3933,7 +4244,7 @@
       <c r="E55" s="14"/>
       <c r="I55" s="14">
         <f>AVERAGE(I21:I40)</f>
-        <v>0.98539049999999995</v>
+        <v>1.1270134999999999</v>
       </c>
       <c r="P55" s="25"/>
       <c r="Z55" s="14">
@@ -3947,7 +4258,7 @@
       </c>
       <c r="I56" s="14">
         <f>AVERAGE(I42:I51)</f>
-        <v>1.4037840000000001</v>
+        <v>1.4295910000000001</v>
       </c>
       <c r="P56" s="25"/>
       <c r="Z56" s="14">
@@ -3964,7 +4275,7 @@
       </c>
       <c r="J58" s="24">
         <f>SUM(J21:J51) / (30*100)</f>
-        <v>0.95899999999999996</v>
+        <v>0.95433333333333337</v>
       </c>
       <c r="P58" s="25"/>
       <c r="AA58" s="24">
@@ -4016,30 +4327,30 @@
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A63" s="7"/>
-      <c r="B63" s="31" t="s">
+      <c r="B63" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="31" t="s">
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="G63" s="33"/>
+      <c r="G63" s="35"/>
       <c r="I63" s="14"/>
       <c r="J63" s="6"/>
       <c r="P63" s="25"/>
       <c r="R63" s="7"/>
-      <c r="S63" s="31" t="s">
+      <c r="S63" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="T63" s="32"/>
-      <c r="U63" s="32"/>
-      <c r="V63" s="33"/>
-      <c r="W63" s="31" t="s">
+      <c r="T63" s="34"/>
+      <c r="U63" s="34"/>
+      <c r="V63" s="35"/>
+      <c r="W63" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="X63" s="33"/>
+      <c r="X63" s="35"/>
       <c r="Z63" s="14"/>
       <c r="AA63" s="6"/>
     </row>
@@ -4400,7 +4711,7 @@
       </c>
       <c r="H71" s="10"/>
       <c r="I71" s="10">
-        <f t="shared" ref="I71" si="6">AVERAGE(F71:G71)</f>
+        <f t="shared" ref="I71" si="8">AVERAGE(F71:G71)</f>
         <v>4.43</v>
       </c>
       <c r="J71" s="12"/>
@@ -4420,7 +4731,7 @@
       </c>
       <c r="Y71" s="10"/>
       <c r="Z71" s="10">
-        <f t="shared" ref="Z71" si="7">AVERAGE(W71:X71)</f>
+        <f t="shared" ref="Z71" si="9">AVERAGE(W71:X71)</f>
         <v>5.91</v>
       </c>
       <c r="AA71" s="12"/>
@@ -4482,7 +4793,7 @@
       </c>
       <c r="H73" s="10"/>
       <c r="I73" s="10">
-        <f t="shared" ref="I73:I74" si="8">AVERAGE(F73:G73)</f>
+        <f t="shared" ref="I73:I74" si="10">AVERAGE(F73:G73)</f>
         <v>4.5150000000000006</v>
       </c>
       <c r="J73" s="12"/>
@@ -4502,7 +4813,7 @@
       </c>
       <c r="Y73" s="10"/>
       <c r="Z73" s="10">
-        <f t="shared" ref="Z73:Z74" si="9">AVERAGE(W73:X73)</f>
+        <f t="shared" ref="Z73:Z74" si="11">AVERAGE(W73:X73)</f>
         <v>6.0250000000000004</v>
       </c>
       <c r="AA73" s="12"/>
@@ -4523,7 +4834,7 @@
       </c>
       <c r="H74" s="11"/>
       <c r="I74" s="11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.5</v>
       </c>
       <c r="J74" s="13"/>
@@ -4543,7 +4854,7 @@
       </c>
       <c r="Y74" s="11"/>
       <c r="Z74" s="11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>5.9350000000000005</v>
       </c>
       <c r="AA74" s="13"/>
@@ -5890,11 +6201,11 @@
         <v>91</v>
       </c>
       <c r="M99" s="10">
-        <f t="shared" ref="M99:M113" si="10">COUNTIF($J$83:$J$113,L99)</f>
+        <f t="shared" ref="M99:M113" si="12">COUNTIF($J$83:$J$113,L99)</f>
         <v>1</v>
       </c>
       <c r="N99" s="24">
-        <f t="shared" ref="N99:N123" si="11">M99/$M$125</f>
+        <f t="shared" ref="N99:N123" si="13">M99/$M$125</f>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P99" s="25"/>
@@ -5975,11 +6286,11 @@
         <v>90</v>
       </c>
       <c r="M100" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N100" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P100" s="25"/>
@@ -6060,11 +6371,11 @@
         <v>89</v>
       </c>
       <c r="M101" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N101" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P101" s="25"/>
@@ -6145,11 +6456,11 @@
         <v>87</v>
       </c>
       <c r="M102" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N102" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P102" s="25"/>
@@ -6170,7 +6481,7 @@
         <v>3</v>
       </c>
       <c r="AE102" s="24">
-        <f t="shared" ref="AE98:AE113" si="12">AD102/$AD$115</f>
+        <f t="shared" ref="AE102:AE111" si="14">AD102/$AD$115</f>
         <v>0.1</v>
       </c>
     </row>
@@ -6188,11 +6499,11 @@
         <v>86</v>
       </c>
       <c r="M103" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N103" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P103" s="25"/>
@@ -6234,7 +6545,7 @@
         <v>5</v>
       </c>
       <c r="AE103" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.16666666666666666</v>
       </c>
     </row>
@@ -6273,11 +6584,11 @@
         <v>83</v>
       </c>
       <c r="M104" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N104" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P104" s="25"/>
@@ -6319,7 +6630,7 @@
         <v>1</v>
       </c>
       <c r="AE104" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
@@ -6358,11 +6669,11 @@
         <v>81</v>
       </c>
       <c r="M105" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N105" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P105" s="25"/>
@@ -6404,7 +6715,7 @@
         <v>1</v>
       </c>
       <c r="AE105" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
@@ -6443,11 +6754,11 @@
         <v>80</v>
       </c>
       <c r="M106" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N106" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P106" s="25"/>
@@ -6489,7 +6800,7 @@
         <v>1</v>
       </c>
       <c r="AE106" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
@@ -6528,11 +6839,11 @@
         <v>76</v>
       </c>
       <c r="M107" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N107" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P107" s="25"/>
@@ -6574,7 +6885,7 @@
         <v>3</v>
       </c>
       <c r="AE107" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.1</v>
       </c>
     </row>
@@ -6613,11 +6924,11 @@
         <v>72</v>
       </c>
       <c r="M108" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N108" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P108" s="25"/>
@@ -6659,7 +6970,7 @@
         <v>2</v>
       </c>
       <c r="AE108" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
@@ -6698,11 +7009,11 @@
         <v>70</v>
       </c>
       <c r="M109" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N109" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P109" s="25"/>
@@ -6744,7 +7055,7 @@
         <v>2</v>
       </c>
       <c r="AE109" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
@@ -6783,11 +7094,11 @@
         <v>69</v>
       </c>
       <c r="M110" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N110" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P110" s="25"/>
@@ -6829,7 +7140,7 @@
         <v>1</v>
       </c>
       <c r="AE110" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
@@ -6868,11 +7179,11 @@
         <v>68</v>
       </c>
       <c r="M111" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="N111" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="P111" s="25"/>
@@ -6914,7 +7225,7 @@
         <v>0</v>
       </c>
       <c r="AE111" s="24">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -6953,11 +7264,11 @@
         <v>67</v>
       </c>
       <c r="M112" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N112" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P112" s="25"/>
@@ -7030,11 +7341,11 @@
         <v>66</v>
       </c>
       <c r="M113" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="N113" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P113" s="25"/>
@@ -7069,7 +7380,7 @@
         <v>1</v>
       </c>
       <c r="N114" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P114" s="25"/>
@@ -7085,15 +7396,15 @@
         <v>19.039333333333335</v>
       </c>
       <c r="U114" s="10">
-        <f t="shared" ref="U114:Y114" si="13">AVERAGE(U82:U101,U103:U112)</f>
+        <f t="shared" ref="U114:W114" si="15">AVERAGE(U82:U101,U103:U112)</f>
         <v>21.762333333333331</v>
       </c>
       <c r="V114" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>13.007999999999999</v>
       </c>
       <c r="W114" s="10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>9.0519999999999996</v>
       </c>
       <c r="X114" s="10">
@@ -7123,23 +7434,23 @@
         <v>44.513666666666673</v>
       </c>
       <c r="D115" s="10">
-        <f t="shared" ref="D115:H115" si="14">AVERAGE(D83:D102,D104:D113)</f>
+        <f t="shared" ref="D115:H115" si="16">AVERAGE(D83:D102,D104:D113)</f>
         <v>0</v>
       </c>
       <c r="E115" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="F115" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="G115" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="H115" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I115" s="10"/>
@@ -7151,11 +7462,11 @@
         <v>61</v>
       </c>
       <c r="M115" s="10">
-        <f t="shared" ref="M115:M123" si="15">COUNTIF($J$83:$J$113,L115)</f>
+        <f t="shared" ref="M115:M123" si="17">COUNTIF($J$83:$J$113,L115)</f>
         <v>1</v>
       </c>
       <c r="N115" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P115" s="25"/>
@@ -7173,11 +7484,11 @@
         <v>50</v>
       </c>
       <c r="M116" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="N116" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="P116" s="25"/>
@@ -7198,11 +7509,11 @@
         <v>48</v>
       </c>
       <c r="M117" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="N117" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P117" s="25"/>
@@ -7223,11 +7534,11 @@
         <v>46</v>
       </c>
       <c r="M118" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="N118" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P118" s="25"/>
@@ -7240,17 +7551,17 @@
         <v>44</v>
       </c>
       <c r="M119" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="N119" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="P119" s="25"/>
       <c r="AA119" s="24">
-        <f>SUM(AA82:AA112) / (30*100)</f>
-        <v>2.3993333333333333</v>
+        <f>SUM(AA82:AA112) / (30*250)</f>
+        <v>0.95973333333333333</v>
       </c>
     </row>
     <row r="120" spans="1:31" x14ac:dyDescent="0.35">
@@ -7264,11 +7575,11 @@
         <v>42</v>
       </c>
       <c r="M120" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="N120" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="P120" s="25"/>
@@ -7278,11 +7589,11 @@
         <v>41</v>
       </c>
       <c r="M121" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="N121" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P121" s="25"/>
@@ -7292,11 +7603,11 @@
         <v>35</v>
       </c>
       <c r="M122" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="N122" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="P122" s="25"/>
@@ -7306,11 +7617,11 @@
         <v>0</v>
       </c>
       <c r="M123" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="N123" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P123" s="25"/>
@@ -7365,35 +7676,45 @@
       <c r="AD128" s="27"/>
       <c r="AE128" s="27"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.35">
       <c r="P129" s="25"/>
-    </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q129" s="32"/>
+      <c r="R129" s="32"/>
+      <c r="S129" s="32"/>
+      <c r="T129" s="32"/>
+      <c r="U129" s="32"/>
+      <c r="V129" s="32"/>
+      <c r="W129" s="32"/>
+      <c r="X129" s="32"/>
+      <c r="Y129" s="32"/>
+      <c r="Z129" s="32"/>
+      <c r="AA129" s="32"/>
+    </row>
+    <row r="130" spans="1:27" x14ac:dyDescent="0.35">
       <c r="P130" s="25"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>85</v>
       </c>
-      <c r="P131" s="25"/>
-    </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="132" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A132" s="7"/>
-      <c r="B132" s="31" t="s">
+      <c r="B132" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C132" s="32"/>
-      <c r="D132" s="32"/>
-      <c r="E132" s="33"/>
-      <c r="F132" s="31" t="s">
+      <c r="C132" s="34"/>
+      <c r="D132" s="34"/>
+      <c r="E132" s="35"/>
+      <c r="F132" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="G132" s="33"/>
+      <c r="G132" s="35"/>
       <c r="I132" s="14"/>
       <c r="J132" s="6"/>
-      <c r="P132" s="25"/>
-    </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="X132" s="14"/>
+    </row>
+    <row r="133" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
         <v>0</v>
       </c>
@@ -7429,9 +7750,13 @@
       <c r="N133" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="P133" s="25"/>
-    </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S133" s="10"/>
+      <c r="T133" s="10"/>
+      <c r="U133" s="10"/>
+      <c r="V133" s="10"/>
+      <c r="X133" s="10"/>
+    </row>
+    <row r="134" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A134" s="6" t="s">
         <v>63</v>
       </c>
@@ -7460,16 +7785,16 @@
         <v>100</v>
       </c>
       <c r="M134" s="10">
-        <f>COUNTIF($J$150:$J$168,L134)</f>
+        <f t="shared" ref="M134:M142" si="18">COUNTIF($J$150:$J$168,L134)</f>
         <v>3</v>
       </c>
       <c r="N134" s="24">
         <f>M134/$M$145</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P134" s="25"/>
-    </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S134" s="1"/>
+    </row>
+    <row r="135" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A135" s="6" t="s">
         <v>61</v>
       </c>
@@ -7497,16 +7822,16 @@
         <v>99</v>
       </c>
       <c r="M135" s="10">
-        <f>COUNTIF($J$150:$J$168,L135)</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="N135" s="24">
-        <f t="shared" ref="N135:N142" si="16">M135/$M$145</f>
+        <f t="shared" ref="N135:N142" si="19">M135/$M$145</f>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="P135" s="25"/>
-    </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S135" s="1"/>
+    </row>
+    <row r="136" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A136" s="6" t="s">
         <v>62</v>
       </c>
@@ -7534,16 +7859,16 @@
         <v>98</v>
       </c>
       <c r="M136" s="10">
-        <f>COUNTIF($J$150:$J$168,L136)</f>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="N136" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="P136" s="25"/>
-    </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S136" s="1"/>
+    </row>
+    <row r="137" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A137" s="6"/>
       <c r="B137" s="10"/>
       <c r="C137" s="10"/>
@@ -7558,16 +7883,16 @@
         <v>97</v>
       </c>
       <c r="M137" s="10">
-        <f>COUNTIF($J$150:$J$168,L137)</f>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="N137" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="P137" s="25"/>
-    </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S137" s="1"/>
+    </row>
+    <row r="138" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A138" s="7"/>
       <c r="B138" s="11"/>
       <c r="C138" s="11"/>
@@ -7582,16 +7907,15 @@
         <v>96</v>
       </c>
       <c r="M138" s="10">
-        <f>COUNTIF($J$150:$J$168,L138)</f>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="N138" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P138" s="25"/>
-    </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A139" s="6" t="s">
         <v>64</v>
       </c>
@@ -7615,16 +7939,16 @@
         <v>94</v>
       </c>
       <c r="M139" s="10">
-        <f>COUNTIF($J$150:$J$168,L139)</f>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="N139" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P139" s="25"/>
-    </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="S139" s="10"/>
+    </row>
+    <row r="140" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A140" s="6" t="s">
         <v>65</v>
       </c>
@@ -7640,7 +7964,7 @@
       </c>
       <c r="H140" s="10"/>
       <c r="I140" s="10">
-        <f t="shared" ref="I140" si="17">AVERAGE(F140:G140)</f>
+        <f t="shared" ref="I140" si="20">AVERAGE(F140:G140)</f>
         <v>6.1099999999999994</v>
       </c>
       <c r="J140" s="12"/>
@@ -7648,16 +7972,15 @@
         <v>92</v>
       </c>
       <c r="M140" s="10">
-        <f>COUNTIF($J$150:$J$168,L140)</f>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="N140" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="P140" s="25"/>
-    </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A141" s="6" t="s">
         <v>66</v>
       </c>
@@ -7681,16 +8004,15 @@
         <v>91</v>
       </c>
       <c r="M141" s="10">
-        <f>COUNTIF($J$150:$J$168,L141)</f>
+        <f t="shared" si="18"/>
         <v>3</v>
       </c>
       <c r="N141" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="19"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="P141" s="25"/>
-    </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.35">
+    </row>
+    <row r="142" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A142" s="6"/>
       <c r="B142" s="10"/>
       <c r="C142" s="10"/>
@@ -7705,15 +8027,15 @@
         <v>0</v>
       </c>
       <c r="M142" s="10">
-        <f>COUNTIF($J$150:$J$168,L142)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="N142" s="24">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.35">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A143" s="7"/>
       <c r="B143" s="11"/>
       <c r="C143" s="11"/>
@@ -7728,7 +8050,7 @@
       <c r="M143" s="10"/>
       <c r="N143" s="24"/>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A144" s="6"/>
       <c r="B144" s="10"/>
       <c r="C144" s="10"/>
@@ -7742,8 +8064,17 @@
       <c r="L144" s="10"/>
       <c r="M144" s="10"/>
       <c r="N144" s="24"/>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="S144" s="1"/>
+      <c r="T144" s="1"/>
+      <c r="U144" s="1"/>
+      <c r="V144" s="1"/>
+      <c r="W144" s="1"/>
+      <c r="X144" s="1"/>
+      <c r="Y144" s="1"/>
+      <c r="Z144" s="10"/>
+      <c r="AA144" s="10"/>
+    </row>
+    <row r="145" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A145" s="6" t="s">
         <v>49</v>
       </c>
@@ -7783,8 +8114,17 @@
         <v>18</v>
       </c>
       <c r="N145" s="24"/>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="S145" s="10"/>
+      <c r="T145" s="10"/>
+      <c r="U145" s="10"/>
+      <c r="V145" s="10"/>
+      <c r="W145" s="10"/>
+      <c r="X145" s="10"/>
+      <c r="Y145" s="10"/>
+      <c r="Z145" s="10"/>
+      <c r="AA145" s="10"/>
+    </row>
+    <row r="146" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A146" s="7"/>
       <c r="B146" s="11"/>
       <c r="C146" s="11"/>
@@ -7798,8 +8138,17 @@
       <c r="L146" s="10"/>
       <c r="M146" s="10"/>
       <c r="N146" s="24"/>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="S146" s="10"/>
+      <c r="T146" s="10"/>
+      <c r="U146" s="10"/>
+      <c r="V146" s="10"/>
+      <c r="W146" s="10"/>
+      <c r="X146" s="10"/>
+      <c r="Y146" s="10"/>
+      <c r="Z146" s="10"/>
+      <c r="AA146" s="10"/>
+    </row>
+    <row r="147" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A147" s="6"/>
       <c r="B147" s="14"/>
       <c r="C147" s="14"/>
@@ -7813,13 +8162,31 @@
       <c r="L147" s="10"/>
       <c r="M147" s="10"/>
       <c r="N147" s="24"/>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="S147" s="10"/>
+      <c r="T147" s="10"/>
+      <c r="U147" s="10"/>
+      <c r="V147" s="10"/>
+      <c r="W147" s="10"/>
+      <c r="X147" s="10"/>
+      <c r="Y147" s="10"/>
+      <c r="Z147" s="10"/>
+      <c r="AA147" s="10"/>
+    </row>
+    <row r="148" spans="1:27" x14ac:dyDescent="0.35">
       <c r="L148" s="10"/>
       <c r="M148" s="10"/>
       <c r="N148" s="24"/>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="S148" s="10"/>
+      <c r="T148" s="10"/>
+      <c r="U148" s="10"/>
+      <c r="V148" s="10"/>
+      <c r="W148" s="10"/>
+      <c r="X148" s="10"/>
+      <c r="Y148" s="10"/>
+      <c r="Z148" s="10"/>
+      <c r="AA148" s="10"/>
+    </row>
+    <row r="149" spans="1:27" x14ac:dyDescent="0.35">
       <c r="B149" s="2">
         <v>4</v>
       </c>
@@ -7850,8 +8217,17 @@
       <c r="L149" s="10"/>
       <c r="M149" s="10"/>
       <c r="N149" s="24"/>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="S149" s="14"/>
+      <c r="T149" s="14"/>
+      <c r="U149" s="14"/>
+      <c r="V149" s="14"/>
+      <c r="W149" s="14"/>
+      <c r="X149" s="14"/>
+      <c r="Y149" s="14"/>
+      <c r="Z149" s="14"/>
+      <c r="AA149" s="14"/>
+    </row>
+    <row r="150" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>67</v>
       </c>
@@ -7886,7 +8262,7 @@
       <c r="M150" s="10"/>
       <c r="N150" s="24"/>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>68</v>
       </c>
@@ -7921,7 +8297,7 @@
       <c r="M151" s="10"/>
       <c r="N151" s="24"/>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>69</v>
       </c>
@@ -7956,7 +8332,7 @@
       <c r="M152" s="10"/>
       <c r="N152" s="24"/>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>70</v>
       </c>
@@ -7991,7 +8367,7 @@
       <c r="M153" s="10"/>
       <c r="N153" s="24"/>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>71</v>
       </c>
@@ -8026,7 +8402,7 @@
       <c r="M154" s="10"/>
       <c r="N154" s="24"/>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>72</v>
       </c>
@@ -8061,7 +8437,7 @@
       <c r="M155" s="10"/>
       <c r="N155" s="24"/>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>73</v>
       </c>
@@ -8096,7 +8472,7 @@
       <c r="M156" s="10"/>
       <c r="N156" s="24"/>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>74</v>
       </c>
@@ -8131,7 +8507,7 @@
       <c r="M157" s="10"/>
       <c r="N157" s="24"/>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>75</v>
       </c>
@@ -8166,7 +8542,7 @@
       <c r="M158" s="10"/>
       <c r="N158" s="24"/>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>76</v>
       </c>
@@ -8201,7 +8577,7 @@
       <c r="M159" s="10"/>
       <c r="N159" s="24"/>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>77</v>
       </c>
@@ -8488,27 +8864,27 @@
         <v>29.186111111111106</v>
       </c>
       <c r="C170" s="10">
-        <f t="shared" ref="C170:H170" si="18">AVERAGE(C150:C161,C163:C168)</f>
+        <f t="shared" ref="C170:H170" si="21">AVERAGE(C150:C161,C163:C168)</f>
         <v>18.782777777777778</v>
       </c>
       <c r="D170" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>21.805555555555557</v>
       </c>
       <c r="E170" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>13.226111111111114</v>
       </c>
       <c r="F170" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>9.5833333333333357</v>
       </c>
       <c r="G170" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>5.2172222222222224</v>
       </c>
       <c r="H170" s="10">
-        <f t="shared" si="18"/>
+        <f t="shared" si="21"/>
         <v>2.1966666666666672</v>
       </c>
       <c r="I170" s="10"/>

</xml_diff>

<commit_message>
final stats and restructure
</commit_message>
<xml_diff>
--- a/Documents/Stats.xlsx
+++ b/Documents/Stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\source\repos\ShadNick\MLPraktikum\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A807F23-8645-48C7-8409-CD23EE5BD021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB86867-3B64-43A9-844F-08756994B801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{C50481C0-3E7F-4500-ADDA-BEE2E952B991}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="98">
   <si>
     <t>Model</t>
   </si>
@@ -335,6 +335,24 @@
   <si>
     <t>Peak Diff Outliner</t>
   </si>
+  <si>
+    <t>Forest Classifier Cancer</t>
+  </si>
+  <si>
+    <t>Forest Classifier Iris</t>
+  </si>
+  <si>
+    <t>Forest Classifier Digits</t>
+  </si>
+  <si>
+    <t>Forest Classifier Wine</t>
+  </si>
+  <si>
+    <t>Forest Regressor Diabetes</t>
+  </si>
+  <si>
+    <t>Forest Regressor Housing</t>
+  </si>
 </sst>
 </file>
 
@@ -488,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,6 +576,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -901,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E18C823A-5B43-45CA-919F-52C1C837F365}">
-  <dimension ref="A1:AE173"/>
+  <dimension ref="A1:AE217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="D175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M201" sqref="M201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -920,6 +942,7 @@
     <col min="18" max="18" width="25.1796875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.35">
@@ -937,16 +960,16 @@
       <c r="I1" s="14"/>
       <c r="J1" s="6"/>
       <c r="R1" s="7"/>
-      <c r="S1" s="33" t="s">
+      <c r="S1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="T1" s="34"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="33" t="s">
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="35"/>
+      <c r="X1" s="37"/>
       <c r="Z1" s="14"/>
       <c r="AA1" s="6"/>
     </row>
@@ -4327,30 +4350,30 @@
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A63" s="7"/>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="33" t="s">
+      <c r="C63" s="36"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="G63" s="35"/>
+      <c r="G63" s="37"/>
       <c r="I63" s="14"/>
       <c r="J63" s="6"/>
       <c r="P63" s="25"/>
       <c r="R63" s="7"/>
-      <c r="S63" s="33" t="s">
+      <c r="S63" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="T63" s="34"/>
-      <c r="U63" s="34"/>
-      <c r="V63" s="35"/>
-      <c r="W63" s="33" t="s">
+      <c r="T63" s="36"/>
+      <c r="U63" s="36"/>
+      <c r="V63" s="37"/>
+      <c r="W63" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="X63" s="35"/>
+      <c r="X63" s="37"/>
       <c r="Z63" s="14"/>
       <c r="AA63" s="6"/>
     </row>
@@ -7697,22 +7720,36 @@
       <c r="A131" t="s">
         <v>85</v>
       </c>
+      <c r="P131" s="25"/>
     </row>
     <row r="132" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A132" s="7"/>
-      <c r="B132" s="33" t="s">
+      <c r="B132" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="C132" s="34"/>
-      <c r="D132" s="34"/>
-      <c r="E132" s="35"/>
-      <c r="F132" s="33" t="s">
+      <c r="C132" s="36"/>
+      <c r="D132" s="36"/>
+      <c r="E132" s="37"/>
+      <c r="F132" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="G132" s="35"/>
+      <c r="G132" s="37"/>
       <c r="I132" s="14"/>
       <c r="J132" s="6"/>
-      <c r="X132" s="14"/>
+      <c r="P132" s="25"/>
+      <c r="R132" s="7"/>
+      <c r="S132" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T132" s="2"/>
+      <c r="U132" s="2"/>
+      <c r="V132" s="3"/>
+      <c r="W132" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="X132" s="18"/>
+      <c r="Z132" s="14"/>
+      <c r="AA132" s="6"/>
     </row>
     <row r="133" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A133" s="5" t="s">
@@ -7750,11 +7787,33 @@
       <c r="N133" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="S133" s="10"/>
-      <c r="T133" s="10"/>
-      <c r="U133" s="10"/>
-      <c r="V133" s="10"/>
-      <c r="X133" s="10"/>
+      <c r="P133" s="25"/>
+      <c r="R133" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S133" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T133" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U133" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V133" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="W133" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="X133" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y133" s="4"/>
+      <c r="Z133" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA133" s="7"/>
     </row>
     <row r="134" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A134" s="6" t="s">
@@ -7792,7 +7851,30 @@
         <f>M134/$M$145</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="S134" s="1"/>
+      <c r="P134" s="25"/>
+      <c r="R134" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S134" s="10">
+        <v>5.85</v>
+      </c>
+      <c r="T134" s="10">
+        <v>5.9</v>
+      </c>
+      <c r="U134" s="10">
+        <v>6.06</v>
+      </c>
+      <c r="V134" s="12">
+        <v>5.89</v>
+      </c>
+      <c r="W134" s="20"/>
+      <c r="X134" s="12"/>
+      <c r="Y134" s="10"/>
+      <c r="Z134" s="10">
+        <f t="shared" ref="Z134:Z141" si="19">AVERAGE(S134:V134)</f>
+        <v>5.9249999999999998</v>
+      </c>
+      <c r="AA134" s="12"/>
     </row>
     <row r="135" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A135" s="6" t="s">
@@ -7826,10 +7908,33 @@
         <v>1</v>
       </c>
       <c r="N135" s="24">
-        <f t="shared" ref="N135:N142" si="19">M135/$M$145</f>
+        <f t="shared" ref="N135:N142" si="20">M135/$M$145</f>
         <v>5.5555555555555552E-2</v>
       </c>
-      <c r="S135" s="1"/>
+      <c r="P135" s="25"/>
+      <c r="R135" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="S135" s="10">
+        <v>5.92</v>
+      </c>
+      <c r="T135" s="10">
+        <v>6.14</v>
+      </c>
+      <c r="U135" s="10">
+        <v>6.34</v>
+      </c>
+      <c r="V135" s="12">
+        <v>5.75</v>
+      </c>
+      <c r="W135" s="20"/>
+      <c r="X135" s="12"/>
+      <c r="Y135" s="10"/>
+      <c r="Z135" s="10">
+        <f t="shared" si="19"/>
+        <v>6.0374999999999996</v>
+      </c>
+      <c r="AA135" s="12"/>
     </row>
     <row r="136" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A136" s="6" t="s">
@@ -7863,10 +7968,33 @@
         <v>2</v>
       </c>
       <c r="N136" s="24">
+        <f t="shared" si="20"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="P136" s="25"/>
+      <c r="R136" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="S136" s="10">
+        <v>6.14</v>
+      </c>
+      <c r="T136" s="10">
+        <v>5.65</v>
+      </c>
+      <c r="U136" s="10">
+        <v>6.2</v>
+      </c>
+      <c r="V136" s="12">
+        <v>5.47</v>
+      </c>
+      <c r="W136" s="20"/>
+      <c r="X136" s="12"/>
+      <c r="Y136" s="10"/>
+      <c r="Z136" s="10">
         <f t="shared" si="19"/>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="S136" s="1"/>
+        <v>5.8649999999999993</v>
+      </c>
+      <c r="AA136" s="12"/>
     </row>
     <row r="137" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A137" s="6"/>
@@ -7887,10 +8015,33 @@
         <v>2</v>
       </c>
       <c r="N137" s="24">
+        <f t="shared" si="20"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="P137" s="25"/>
+      <c r="R137" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="S137" s="10">
+        <v>5.77</v>
+      </c>
+      <c r="T137" s="10">
+        <v>5.29</v>
+      </c>
+      <c r="U137" s="10">
+        <v>5.91</v>
+      </c>
+      <c r="V137" s="12">
+        <v>5.99</v>
+      </c>
+      <c r="W137" s="10"/>
+      <c r="X137" s="12"/>
+      <c r="Y137" s="10"/>
+      <c r="Z137" s="10">
         <f t="shared" si="19"/>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="S137" s="1"/>
+        <v>5.74</v>
+      </c>
+      <c r="AA137" s="12"/>
     </row>
     <row r="138" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A138" s="7"/>
@@ -7911,9 +8062,33 @@
         <v>3</v>
       </c>
       <c r="N138" s="24">
+        <f t="shared" si="20"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P138" s="25"/>
+      <c r="R138" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="S138" s="10">
+        <v>5.72</v>
+      </c>
+      <c r="T138" s="10">
+        <v>5.42</v>
+      </c>
+      <c r="U138" s="10">
+        <v>5.85</v>
+      </c>
+      <c r="V138" s="12">
+        <v>5.56</v>
+      </c>
+      <c r="W138" s="10"/>
+      <c r="X138" s="12"/>
+      <c r="Y138" s="10"/>
+      <c r="Z138" s="10">
         <f t="shared" si="19"/>
-        <v>0.16666666666666666</v>
-      </c>
+        <v>5.6375000000000002</v>
+      </c>
+      <c r="AA138" s="12"/>
     </row>
     <row r="139" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A139" s="6" t="s">
@@ -7943,10 +8118,31 @@
         <v>3</v>
       </c>
       <c r="N139" s="24">
+        <f t="shared" si="20"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P139" s="25"/>
+      <c r="R139" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="S139" s="1">
+        <v>6.18</v>
+      </c>
+      <c r="T139" s="1">
+        <v>5.69</v>
+      </c>
+      <c r="U139" s="1">
+        <v>6.11</v>
+      </c>
+      <c r="V139" s="34">
+        <v>5.27</v>
+      </c>
+      <c r="X139" s="6"/>
+      <c r="Z139" s="10">
         <f t="shared" si="19"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="S139" s="10"/>
+        <v>5.8125</v>
+      </c>
+      <c r="AA139" s="6"/>
     </row>
     <row r="140" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A140" s="6" t="s">
@@ -7964,7 +8160,7 @@
       </c>
       <c r="H140" s="10"/>
       <c r="I140" s="10">
-        <f t="shared" ref="I140" si="20">AVERAGE(F140:G140)</f>
+        <f t="shared" ref="I140" si="21">AVERAGE(F140:G140)</f>
         <v>6.1099999999999994</v>
       </c>
       <c r="J140" s="12"/>
@@ -7976,9 +8172,31 @@
         <v>1</v>
       </c>
       <c r="N140" s="24">
+        <f t="shared" si="20"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="P140" s="25"/>
+      <c r="R140" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="S140" s="1">
+        <v>5.64</v>
+      </c>
+      <c r="T140" s="1">
+        <v>5.36</v>
+      </c>
+      <c r="U140" s="1">
+        <v>5.85</v>
+      </c>
+      <c r="V140" s="34">
+        <v>5.85</v>
+      </c>
+      <c r="X140" s="6"/>
+      <c r="Z140" s="10">
         <f t="shared" si="19"/>
-        <v>5.5555555555555552E-2</v>
-      </c>
+        <v>5.6750000000000007</v>
+      </c>
+      <c r="AA140" s="6"/>
     </row>
     <row r="141" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A141" s="6" t="s">
@@ -8008,9 +8226,33 @@
         <v>3</v>
       </c>
       <c r="N141" s="24">
+        <f t="shared" si="20"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P141" s="25"/>
+      <c r="R141" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="S141" s="2">
+        <v>5.77</v>
+      </c>
+      <c r="T141" s="2">
+        <v>5.14</v>
+      </c>
+      <c r="U141" s="2">
+        <v>5.98</v>
+      </c>
+      <c r="V141" s="3">
+        <v>5.58</v>
+      </c>
+      <c r="W141" s="4"/>
+      <c r="X141" s="7"/>
+      <c r="Y141" s="4"/>
+      <c r="Z141" s="10">
         <f t="shared" si="19"/>
-        <v>0.16666666666666666</v>
-      </c>
+        <v>5.6174999999999997</v>
+      </c>
+      <c r="AA141" s="7"/>
     </row>
     <row r="142" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A142" s="6"/>
@@ -8031,9 +8273,29 @@
         <v>0</v>
       </c>
       <c r="N142" s="24">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="P142" s="25"/>
+      <c r="R142" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="S142" s="10"/>
+      <c r="T142" s="10"/>
+      <c r="U142" s="10"/>
+      <c r="V142" s="12"/>
+      <c r="W142" s="20">
+        <v>5.96</v>
+      </c>
+      <c r="X142" s="12">
+        <v>6.09</v>
+      </c>
+      <c r="Y142" s="10"/>
+      <c r="Z142" s="10">
+        <f>AVERAGE(W142:X142)</f>
+        <v>6.0250000000000004</v>
+      </c>
+      <c r="AA142" s="12"/>
     </row>
     <row r="143" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A143" s="7"/>
@@ -8049,6 +8311,26 @@
       <c r="L143" s="10"/>
       <c r="M143" s="10"/>
       <c r="N143" s="24"/>
+      <c r="P143" s="25"/>
+      <c r="R143" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="S143" s="10"/>
+      <c r="T143" s="10"/>
+      <c r="U143" s="10"/>
+      <c r="V143" s="12"/>
+      <c r="W143" s="20">
+        <v>5.99</v>
+      </c>
+      <c r="X143" s="12">
+        <v>6.01</v>
+      </c>
+      <c r="Y143" s="10"/>
+      <c r="Z143" s="10">
+        <f>AVERAGE(W143:X143)</f>
+        <v>6</v>
+      </c>
+      <c r="AA143" s="12"/>
     </row>
     <row r="144" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A144" s="6"/>
@@ -8064,17 +8346,28 @@
       <c r="L144" s="10"/>
       <c r="M144" s="10"/>
       <c r="N144" s="24"/>
-      <c r="S144" s="1"/>
-      <c r="T144" s="1"/>
-      <c r="U144" s="1"/>
-      <c r="V144" s="1"/>
-      <c r="W144" s="1"/>
-      <c r="X144" s="1"/>
-      <c r="Y144" s="1"/>
-      <c r="Z144" s="10"/>
-      <c r="AA144" s="10"/>
-    </row>
-    <row r="145" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P144" s="25"/>
+      <c r="R144" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="S144" s="10"/>
+      <c r="T144" s="10"/>
+      <c r="U144" s="10"/>
+      <c r="V144" s="12"/>
+      <c r="W144" s="20">
+        <v>5.76</v>
+      </c>
+      <c r="X144" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="Y144" s="10"/>
+      <c r="Z144" s="10">
+        <f t="shared" ref="Z144:Z149" si="22">AVERAGE(W144:X144)</f>
+        <v>5.875</v>
+      </c>
+      <c r="AA144" s="12"/>
+    </row>
+    <row r="145" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A145" s="6" t="s">
         <v>49</v>
       </c>
@@ -8114,17 +8407,28 @@
         <v>18</v>
       </c>
       <c r="N145" s="24"/>
+      <c r="P145" s="25"/>
+      <c r="R145" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="S145" s="10"/>
       <c r="T145" s="10"/>
       <c r="U145" s="10"/>
-      <c r="V145" s="10"/>
-      <c r="W145" s="10"/>
-      <c r="X145" s="10"/>
+      <c r="V145" s="12"/>
+      <c r="W145" s="10">
+        <v>6.23</v>
+      </c>
+      <c r="X145" s="12">
+        <v>6.11</v>
+      </c>
       <c r="Y145" s="10"/>
-      <c r="Z145" s="10"/>
-      <c r="AA145" s="10"/>
-    </row>
-    <row r="146" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z145" s="10">
+        <f t="shared" si="22"/>
+        <v>6.17</v>
+      </c>
+      <c r="AA145" s="12"/>
+    </row>
+    <row r="146" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A146" s="7"/>
       <c r="B146" s="11"/>
       <c r="C146" s="11"/>
@@ -8138,17 +8442,28 @@
       <c r="L146" s="10"/>
       <c r="M146" s="10"/>
       <c r="N146" s="24"/>
+      <c r="P146" s="25"/>
+      <c r="R146" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="S146" s="10"/>
       <c r="T146" s="10"/>
       <c r="U146" s="10"/>
-      <c r="V146" s="10"/>
-      <c r="W146" s="10"/>
-      <c r="X146" s="10"/>
+      <c r="V146" s="12"/>
+      <c r="W146" s="10">
+        <v>5.82</v>
+      </c>
+      <c r="X146" s="12">
+        <v>6.11</v>
+      </c>
       <c r="Y146" s="10"/>
-      <c r="Z146" s="10"/>
-      <c r="AA146" s="10"/>
-    </row>
-    <row r="147" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z146" s="10">
+        <f t="shared" si="22"/>
+        <v>5.9649999999999999</v>
+      </c>
+      <c r="AA146" s="12"/>
+    </row>
+    <row r="147" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A147" s="6"/>
       <c r="B147" s="14"/>
       <c r="C147" s="14"/>
@@ -8162,31 +8477,45 @@
       <c r="L147" s="10"/>
       <c r="M147" s="10"/>
       <c r="N147" s="24"/>
-      <c r="S147" s="10"/>
-      <c r="T147" s="10"/>
-      <c r="U147" s="10"/>
-      <c r="V147" s="10"/>
-      <c r="W147" s="10"/>
-      <c r="X147" s="10"/>
-      <c r="Y147" s="10"/>
-      <c r="Z147" s="10"/>
-      <c r="AA147" s="10"/>
-    </row>
-    <row r="148" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P147" s="25"/>
+      <c r="R147" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="V147" s="6"/>
+      <c r="W147" s="1">
+        <v>6.03</v>
+      </c>
+      <c r="X147" s="34">
+        <v>5.87</v>
+      </c>
+      <c r="Z147" s="10">
+        <f t="shared" si="22"/>
+        <v>5.95</v>
+      </c>
+      <c r="AA147" s="6"/>
+    </row>
+    <row r="148" spans="1:30" x14ac:dyDescent="0.35">
       <c r="L148" s="10"/>
       <c r="M148" s="10"/>
       <c r="N148" s="24"/>
-      <c r="S148" s="10"/>
-      <c r="T148" s="10"/>
-      <c r="U148" s="10"/>
-      <c r="V148" s="10"/>
-      <c r="W148" s="10"/>
-      <c r="X148" s="10"/>
-      <c r="Y148" s="10"/>
-      <c r="Z148" s="10"/>
-      <c r="AA148" s="10"/>
-    </row>
-    <row r="149" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P148" s="25"/>
+      <c r="R148" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="V148" s="6"/>
+      <c r="W148" s="1">
+        <v>6.02</v>
+      </c>
+      <c r="X148" s="34">
+        <v>6.18</v>
+      </c>
+      <c r="Z148" s="10">
+        <f t="shared" si="22"/>
+        <v>6.1</v>
+      </c>
+      <c r="AA148" s="6"/>
+    </row>
+    <row r="149" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B149" s="2">
         <v>4</v>
       </c>
@@ -8217,17 +8546,28 @@
       <c r="L149" s="10"/>
       <c r="M149" s="10"/>
       <c r="N149" s="24"/>
-      <c r="S149" s="14"/>
-      <c r="T149" s="14"/>
-      <c r="U149" s="14"/>
-      <c r="V149" s="14"/>
-      <c r="W149" s="14"/>
-      <c r="X149" s="14"/>
-      <c r="Y149" s="14"/>
-      <c r="Z149" s="14"/>
-      <c r="AA149" s="14"/>
-    </row>
-    <row r="150" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P149" s="25"/>
+      <c r="R149" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="S149" s="4"/>
+      <c r="T149" s="4"/>
+      <c r="U149" s="4"/>
+      <c r="V149" s="7"/>
+      <c r="W149" s="2">
+        <v>6.03</v>
+      </c>
+      <c r="X149" s="3">
+        <v>5.63</v>
+      </c>
+      <c r="Y149" s="33"/>
+      <c r="Z149" s="11">
+        <f t="shared" si="22"/>
+        <v>5.83</v>
+      </c>
+      <c r="AA149" s="7"/>
+    </row>
+    <row r="150" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>67</v>
       </c>
@@ -8261,8 +8601,19 @@
       <c r="L150" s="10"/>
       <c r="M150" s="10"/>
       <c r="N150" s="24"/>
-    </row>
-    <row r="151" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P150" s="25"/>
+      <c r="R150" s="6"/>
+      <c r="S150" s="10"/>
+      <c r="T150" s="10"/>
+      <c r="U150" s="10"/>
+      <c r="V150" s="21"/>
+      <c r="W150" s="10"/>
+      <c r="X150" s="12"/>
+      <c r="Y150" s="10"/>
+      <c r="Z150" s="10"/>
+      <c r="AA150" s="12"/>
+    </row>
+    <row r="151" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>68</v>
       </c>
@@ -8296,8 +8647,42 @@
       <c r="L151" s="10"/>
       <c r="M151" s="10"/>
       <c r="N151" s="24"/>
-    </row>
-    <row r="152" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P151" s="25"/>
+      <c r="R151" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="S151" s="10">
+        <f>AVERAGE(S134:S141)</f>
+        <v>5.8737499999999994</v>
+      </c>
+      <c r="T151" s="10">
+        <f>AVERAGE(T134:T141)</f>
+        <v>5.5737499999999995</v>
+      </c>
+      <c r="U151" s="10">
+        <f>AVERAGE(U134:U141)</f>
+        <v>6.0374999999999996</v>
+      </c>
+      <c r="V151" s="12">
+        <f>AVERAGE(V134:V142)</f>
+        <v>5.67</v>
+      </c>
+      <c r="W151" s="10">
+        <f>AVERAGE(W142:W149)</f>
+        <v>5.98</v>
+      </c>
+      <c r="X151" s="12">
+        <f>AVERAGE(X142:X149)</f>
+        <v>5.9987500000000002</v>
+      </c>
+      <c r="Y151" s="10"/>
+      <c r="Z151" s="10">
+        <f>AVERAGE(S151:X151,Z134:Z149)</f>
+        <v>5.8799431818181827</v>
+      </c>
+      <c r="AA151" s="12"/>
+    </row>
+    <row r="152" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>69</v>
       </c>
@@ -8331,8 +8716,19 @@
       <c r="L152" s="10"/>
       <c r="M152" s="10"/>
       <c r="N152" s="24"/>
-    </row>
-    <row r="153" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P152" s="25"/>
+      <c r="R152" s="7"/>
+      <c r="S152" s="11"/>
+      <c r="T152" s="11"/>
+      <c r="U152" s="11"/>
+      <c r="V152" s="13"/>
+      <c r="W152" s="11"/>
+      <c r="X152" s="13"/>
+      <c r="Y152" s="11"/>
+      <c r="Z152" s="11"/>
+      <c r="AA152" s="13"/>
+    </row>
+    <row r="153" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>70</v>
       </c>
@@ -8366,8 +8762,19 @@
       <c r="L153" s="10"/>
       <c r="M153" s="10"/>
       <c r="N153" s="24"/>
-    </row>
-    <row r="154" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P153" s="25"/>
+      <c r="R153" s="6"/>
+      <c r="S153" s="14"/>
+      <c r="T153" s="14"/>
+      <c r="U153" s="14"/>
+      <c r="V153" s="15"/>
+      <c r="W153" s="22"/>
+      <c r="X153" s="23"/>
+      <c r="Y153" s="14"/>
+      <c r="Z153" s="14"/>
+      <c r="AA153" s="15"/>
+    </row>
+    <row r="154" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>71</v>
       </c>
@@ -8401,8 +8808,9 @@
       <c r="L154" s="10"/>
       <c r="M154" s="10"/>
       <c r="N154" s="24"/>
-    </row>
-    <row r="155" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P154" s="25"/>
+    </row>
+    <row r="155" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>72</v>
       </c>
@@ -8436,8 +8844,9 @@
       <c r="L155" s="10"/>
       <c r="M155" s="10"/>
       <c r="N155" s="24"/>
-    </row>
-    <row r="156" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P155" s="25"/>
+    </row>
+    <row r="156" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>73</v>
       </c>
@@ -8471,8 +8880,9 @@
       <c r="L156" s="10"/>
       <c r="M156" s="10"/>
       <c r="N156" s="24"/>
-    </row>
-    <row r="157" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P156" s="25"/>
+    </row>
+    <row r="157" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>74</v>
       </c>
@@ -8506,8 +8916,42 @@
       <c r="L157" s="10"/>
       <c r="M157" s="10"/>
       <c r="N157" s="24"/>
-    </row>
-    <row r="158" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P157" s="25"/>
+      <c r="S157" s="2">
+        <v>4</v>
+      </c>
+      <c r="T157" s="2">
+        <v>5</v>
+      </c>
+      <c r="U157" s="2">
+        <v>6</v>
+      </c>
+      <c r="V157" s="2">
+        <v>7</v>
+      </c>
+      <c r="W157" s="2">
+        <v>8</v>
+      </c>
+      <c r="X157" s="2">
+        <v>9</v>
+      </c>
+      <c r="Y157" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z157" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA157" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC157" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AD157" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="158" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>75</v>
       </c>
@@ -8541,8 +8985,45 @@
       <c r="L158" s="10"/>
       <c r="M158" s="10"/>
       <c r="N158" s="24"/>
-    </row>
-    <row r="159" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P158" s="25"/>
+      <c r="R158" t="s">
+        <v>11</v>
+      </c>
+      <c r="S158" s="10">
+        <v>27.84</v>
+      </c>
+      <c r="T158" s="10">
+        <v>20.62</v>
+      </c>
+      <c r="U158" s="10">
+        <v>20.62</v>
+      </c>
+      <c r="V158" s="10">
+        <v>13.4</v>
+      </c>
+      <c r="W158" s="10">
+        <v>6.19</v>
+      </c>
+      <c r="X158" s="10">
+        <v>10.31</v>
+      </c>
+      <c r="Y158" s="10">
+        <v>1.03</v>
+      </c>
+      <c r="Z158" s="10">
+        <v>0.59592999999999996</v>
+      </c>
+      <c r="AA158" s="10">
+        <v>95</v>
+      </c>
+      <c r="AC158" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD158" s="10">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="159" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>76</v>
       </c>
@@ -8576,8 +9057,45 @@
       <c r="L159" s="10"/>
       <c r="M159" s="10"/>
       <c r="N159" s="24"/>
-    </row>
-    <row r="160" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="P159" s="25"/>
+      <c r="R159" t="s">
+        <v>12</v>
+      </c>
+      <c r="S159" s="10">
+        <v>34.340000000000003</v>
+      </c>
+      <c r="T159" s="10">
+        <v>15.15</v>
+      </c>
+      <c r="U159" s="10">
+        <v>14.14</v>
+      </c>
+      <c r="V159" s="10">
+        <v>14.14</v>
+      </c>
+      <c r="W159" s="10">
+        <v>10.1</v>
+      </c>
+      <c r="X159" s="10">
+        <v>9.09</v>
+      </c>
+      <c r="Y159" s="10">
+        <v>3.03</v>
+      </c>
+      <c r="Z159" s="10">
+        <v>1.67604</v>
+      </c>
+      <c r="AA159" s="10">
+        <v>96</v>
+      </c>
+      <c r="AC159" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD159" s="10">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="160" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>77</v>
       </c>
@@ -8608,8 +9126,45 @@
       <c r="J160" s="10">
         <v>100</v>
       </c>
-    </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P160" s="25"/>
+      <c r="R160" t="s">
+        <v>13</v>
+      </c>
+      <c r="S160" s="10">
+        <v>24.74</v>
+      </c>
+      <c r="T160" s="10">
+        <v>17.53</v>
+      </c>
+      <c r="U160" s="10">
+        <v>25.77</v>
+      </c>
+      <c r="V160" s="10">
+        <v>8.25</v>
+      </c>
+      <c r="W160" s="10">
+        <v>12.37</v>
+      </c>
+      <c r="X160" s="10">
+        <v>5.15</v>
+      </c>
+      <c r="Y160" s="10">
+        <v>6.19</v>
+      </c>
+      <c r="Z160" s="10">
+        <v>1.2084900000000001</v>
+      </c>
+      <c r="AA160" s="10">
+        <v>99</v>
+      </c>
+      <c r="AC160" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD160" s="10">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="161" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>78</v>
       </c>
@@ -8640,8 +9195,45 @@
       <c r="J161" s="10">
         <v>96</v>
       </c>
-    </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P161" s="25"/>
+      <c r="R161" t="s">
+        <v>14</v>
+      </c>
+      <c r="S161" s="10">
+        <v>27.27</v>
+      </c>
+      <c r="T161" s="10">
+        <v>18.18</v>
+      </c>
+      <c r="U161" s="10">
+        <v>21.21</v>
+      </c>
+      <c r="V161" s="10">
+        <v>18.18</v>
+      </c>
+      <c r="W161" s="10">
+        <v>6.06</v>
+      </c>
+      <c r="X161" s="10">
+        <v>5.05</v>
+      </c>
+      <c r="Y161" s="10">
+        <v>4.04</v>
+      </c>
+      <c r="Z161" s="10">
+        <v>1.2633300000000001</v>
+      </c>
+      <c r="AA161" s="10">
+        <v>98</v>
+      </c>
+      <c r="AC161" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD161" s="10">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B162" s="10"/>
       <c r="C162" s="10"/>
       <c r="D162" s="10"/>
@@ -8651,8 +9243,45 @@
       <c r="H162" s="10"/>
       <c r="I162" s="10"/>
       <c r="J162" s="10"/>
-    </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P162" s="25"/>
+      <c r="R162" t="s">
+        <v>15</v>
+      </c>
+      <c r="S162" s="10">
+        <v>28.42</v>
+      </c>
+      <c r="T162" s="10">
+        <v>16.84</v>
+      </c>
+      <c r="U162" s="10">
+        <v>24.21</v>
+      </c>
+      <c r="V162" s="10">
+        <v>11.58</v>
+      </c>
+      <c r="W162" s="10">
+        <v>7.37</v>
+      </c>
+      <c r="X162" s="10">
+        <v>7.37</v>
+      </c>
+      <c r="Y162" s="10">
+        <v>4.21</v>
+      </c>
+      <c r="Z162" s="10">
+        <v>0.86580999999999997</v>
+      </c>
+      <c r="AA162" s="10">
+        <v>93</v>
+      </c>
+      <c r="AC162" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD162" s="10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>79</v>
       </c>
@@ -8683,8 +9312,45 @@
       <c r="J163" s="10">
         <v>91</v>
       </c>
-    </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P163" s="25"/>
+      <c r="R163" t="s">
+        <v>16</v>
+      </c>
+      <c r="S163" s="10">
+        <v>28</v>
+      </c>
+      <c r="T163" s="10">
+        <v>13</v>
+      </c>
+      <c r="U163" s="10">
+        <v>18</v>
+      </c>
+      <c r="V163" s="10">
+        <v>16</v>
+      </c>
+      <c r="W163" s="10">
+        <v>13</v>
+      </c>
+      <c r="X163" s="10">
+        <v>7</v>
+      </c>
+      <c r="Y163" s="10">
+        <v>5</v>
+      </c>
+      <c r="Z163" s="10">
+        <v>1.5930599999999999</v>
+      </c>
+      <c r="AA163" s="10">
+        <v>98</v>
+      </c>
+      <c r="AC163" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD163" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>80</v>
       </c>
@@ -8715,8 +9381,45 @@
       <c r="J164" s="10">
         <v>100</v>
       </c>
-    </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P164" s="25"/>
+      <c r="R164" t="s">
+        <v>17</v>
+      </c>
+      <c r="S164" s="10">
+        <v>23.4</v>
+      </c>
+      <c r="T164" s="10">
+        <v>12.77</v>
+      </c>
+      <c r="U164" s="10">
+        <v>22.34</v>
+      </c>
+      <c r="V164" s="10">
+        <v>13.83</v>
+      </c>
+      <c r="W164" s="10">
+        <v>10.64</v>
+      </c>
+      <c r="X164" s="10">
+        <v>9.57</v>
+      </c>
+      <c r="Y164" s="10">
+        <v>7.45</v>
+      </c>
+      <c r="Z164" s="10">
+        <v>0.57608999999999999</v>
+      </c>
+      <c r="AA164" s="10">
+        <v>98</v>
+      </c>
+      <c r="AC164" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD164" s="10">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>81</v>
       </c>
@@ -8747,8 +9450,45 @@
       <c r="J165" s="10">
         <v>96</v>
       </c>
-    </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P165" s="25"/>
+      <c r="R165" t="s">
+        <v>18</v>
+      </c>
+      <c r="S165" s="10">
+        <v>35.35</v>
+      </c>
+      <c r="T165" s="10">
+        <v>14.14</v>
+      </c>
+      <c r="U165" s="10">
+        <v>18.18</v>
+      </c>
+      <c r="V165" s="10">
+        <v>16.16</v>
+      </c>
+      <c r="W165" s="10">
+        <v>9.09</v>
+      </c>
+      <c r="X165" s="10">
+        <v>3.03</v>
+      </c>
+      <c r="Y165" s="10">
+        <v>4.04</v>
+      </c>
+      <c r="Z165" s="10">
+        <v>1.91473</v>
+      </c>
+      <c r="AA165" s="10">
+        <v>92</v>
+      </c>
+      <c r="AC165" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD165" s="10">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="166" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>82</v>
       </c>
@@ -8779,8 +9519,45 @@
       <c r="J166" s="10">
         <v>94</v>
       </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P166" s="25"/>
+      <c r="R166" t="s">
+        <v>19</v>
+      </c>
+      <c r="S166" s="10">
+        <v>23.16</v>
+      </c>
+      <c r="T166" s="10">
+        <v>21.05</v>
+      </c>
+      <c r="U166" s="10">
+        <v>15.79</v>
+      </c>
+      <c r="V166" s="10">
+        <v>14.74</v>
+      </c>
+      <c r="W166" s="10">
+        <v>12.63</v>
+      </c>
+      <c r="X166" s="10">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="Y166" s="10">
+        <v>3.16</v>
+      </c>
+      <c r="Z166" s="10">
+        <v>0.75204000000000004</v>
+      </c>
+      <c r="AA166" s="10">
+        <v>93</v>
+      </c>
+      <c r="AC166" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD166" s="10">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>83</v>
       </c>
@@ -8811,8 +9588,45 @@
       <c r="J167" s="10">
         <v>96</v>
       </c>
-    </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P167" s="25"/>
+      <c r="R167" t="s">
+        <v>20</v>
+      </c>
+      <c r="S167" s="10">
+        <v>33.33</v>
+      </c>
+      <c r="T167" s="10">
+        <v>9.09</v>
+      </c>
+      <c r="U167" s="10">
+        <v>31.31</v>
+      </c>
+      <c r="V167" s="10">
+        <v>15.15</v>
+      </c>
+      <c r="W167" s="10">
+        <v>9.09</v>
+      </c>
+      <c r="X167" s="10">
+        <v>1.01</v>
+      </c>
+      <c r="Y167" s="10">
+        <v>1.01</v>
+      </c>
+      <c r="Z167" s="10">
+        <v>1.2208399999999999</v>
+      </c>
+      <c r="AA167" s="10">
+        <v>99</v>
+      </c>
+      <c r="AC167" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD167" s="10">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="168" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>84</v>
       </c>
@@ -8843,8 +9657,45 @@
       <c r="J168" s="10">
         <v>100</v>
       </c>
-    </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P168" s="25"/>
+      <c r="R168" t="s">
+        <v>21</v>
+      </c>
+      <c r="S168" s="10">
+        <v>20.62</v>
+      </c>
+      <c r="T168" s="10">
+        <v>19.59</v>
+      </c>
+      <c r="U168" s="10">
+        <v>19.59</v>
+      </c>
+      <c r="V168" s="10">
+        <v>15.46</v>
+      </c>
+      <c r="W168" s="10">
+        <v>14.43</v>
+      </c>
+      <c r="X168" s="10">
+        <v>5.15</v>
+      </c>
+      <c r="Y168" s="10">
+        <v>5.15</v>
+      </c>
+      <c r="Z168" s="10">
+        <v>0.70121999999999995</v>
+      </c>
+      <c r="AA168" s="10">
+        <v>96</v>
+      </c>
+      <c r="AC168" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD168" s="10">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
@@ -8854,8 +9705,45 @@
       <c r="H169" s="1"/>
       <c r="I169" s="1"/>
       <c r="J169" s="10"/>
-    </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P169" s="25"/>
+      <c r="R169" t="s">
+        <v>22</v>
+      </c>
+      <c r="S169" s="10">
+        <v>37</v>
+      </c>
+      <c r="T169" s="10">
+        <v>14</v>
+      </c>
+      <c r="U169" s="10">
+        <v>27</v>
+      </c>
+      <c r="V169" s="10">
+        <v>15</v>
+      </c>
+      <c r="W169" s="10">
+        <v>3</v>
+      </c>
+      <c r="X169" s="10">
+        <v>2</v>
+      </c>
+      <c r="Y169" s="10">
+        <v>2</v>
+      </c>
+      <c r="Z169" s="10">
+        <v>1.1634899999999999</v>
+      </c>
+      <c r="AA169" s="10">
+        <v>96</v>
+      </c>
+      <c r="AC169" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD169" s="10">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="170" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>49</v>
       </c>
@@ -8864,27 +9752,27 @@
         <v>29.186111111111106</v>
       </c>
       <c r="C170" s="10">
-        <f t="shared" ref="C170:H170" si="21">AVERAGE(C150:C161,C163:C168)</f>
+        <f t="shared" ref="C170:H170" si="23">AVERAGE(C150:C161,C163:C168)</f>
         <v>18.782777777777778</v>
       </c>
       <c r="D170" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>21.805555555555557</v>
       </c>
       <c r="E170" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>13.226111111111114</v>
       </c>
       <c r="F170" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>9.5833333333333357</v>
       </c>
       <c r="G170" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>5.2172222222222224</v>
       </c>
       <c r="H170" s="10">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2.1966666666666672</v>
       </c>
       <c r="I170" s="10"/>
@@ -8892,8 +9780,45 @@
         <f>SUM(J150:J168) / (18*100)</f>
         <v>0.95777777777777773</v>
       </c>
-    </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P170" s="25"/>
+      <c r="R170" t="s">
+        <v>89</v>
+      </c>
+      <c r="S170" s="10">
+        <v>29.79</v>
+      </c>
+      <c r="T170" s="10">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="U170" s="10">
+        <v>22.34</v>
+      </c>
+      <c r="V170" s="10">
+        <v>11.7</v>
+      </c>
+      <c r="W170" s="10">
+        <v>9.57</v>
+      </c>
+      <c r="X170" s="10">
+        <v>5.32</v>
+      </c>
+      <c r="Y170" s="10">
+        <v>2.13</v>
+      </c>
+      <c r="Z170" s="10">
+        <v>0.78122999999999998</v>
+      </c>
+      <c r="AA170" s="10">
+        <v>93</v>
+      </c>
+      <c r="AC170" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD170" s="10">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
@@ -8903,8 +9828,45 @@
       <c r="H171" s="1"/>
       <c r="I171" s="1"/>
       <c r="J171" s="10"/>
-    </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P171" s="25"/>
+      <c r="R171" t="s">
+        <v>24</v>
+      </c>
+      <c r="S171" s="10">
+        <v>45</v>
+      </c>
+      <c r="T171" s="10">
+        <v>12</v>
+      </c>
+      <c r="U171" s="10">
+        <v>21</v>
+      </c>
+      <c r="V171" s="10">
+        <v>14</v>
+      </c>
+      <c r="W171" s="10">
+        <v>7</v>
+      </c>
+      <c r="X171" s="10">
+        <v>1</v>
+      </c>
+      <c r="Y171" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z171" s="10">
+        <v>1.4334</v>
+      </c>
+      <c r="AA171" s="10">
+        <v>88</v>
+      </c>
+      <c r="AC171" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD171" s="10">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
@@ -8917,8 +9879,45 @@
         <v>1.9932466666666666</v>
       </c>
       <c r="J172" s="10"/>
-    </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="P172" s="25"/>
+      <c r="R172" t="s">
+        <v>25</v>
+      </c>
+      <c r="S172" s="10">
+        <v>25</v>
+      </c>
+      <c r="T172" s="10">
+        <v>22.92</v>
+      </c>
+      <c r="U172" s="10">
+        <v>17.71</v>
+      </c>
+      <c r="V172" s="10">
+        <v>15.62</v>
+      </c>
+      <c r="W172" s="10">
+        <v>10.42</v>
+      </c>
+      <c r="X172" s="10">
+        <v>6.25</v>
+      </c>
+      <c r="Y172" s="10">
+        <v>2.08</v>
+      </c>
+      <c r="Z172" s="10">
+        <v>0.17602999999999999</v>
+      </c>
+      <c r="AA172" s="10">
+        <v>96</v>
+      </c>
+      <c r="AC172" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD172" s="10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="173" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
@@ -8931,6 +9930,1398 @@
         <v>3.2352249999999998</v>
       </c>
       <c r="J173" s="10"/>
+      <c r="P173" s="25"/>
+      <c r="R173" t="s">
+        <v>26</v>
+      </c>
+      <c r="S173" s="10">
+        <v>22.45</v>
+      </c>
+      <c r="T173" s="10">
+        <v>20.41</v>
+      </c>
+      <c r="U173" s="10">
+        <v>23.47</v>
+      </c>
+      <c r="V173" s="10">
+        <v>14.29</v>
+      </c>
+      <c r="W173" s="10">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="X173" s="10">
+        <v>7.14</v>
+      </c>
+      <c r="Y173" s="10">
+        <v>2.04</v>
+      </c>
+      <c r="Z173" s="10">
+        <v>3.1112099999999998</v>
+      </c>
+      <c r="AA173" s="10">
+        <v>95</v>
+      </c>
+      <c r="AC173" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD173" s="10">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="174" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="P174" s="25"/>
+      <c r="R174" t="s">
+        <v>27</v>
+      </c>
+      <c r="S174" s="10">
+        <v>28.12</v>
+      </c>
+      <c r="T174" s="10">
+        <v>23.96</v>
+      </c>
+      <c r="U174" s="10">
+        <v>17.71</v>
+      </c>
+      <c r="V174" s="10">
+        <v>17.71</v>
+      </c>
+      <c r="W174" s="10">
+        <v>5.21</v>
+      </c>
+      <c r="X174" s="10">
+        <v>5.21</v>
+      </c>
+      <c r="Y174" s="10">
+        <v>2.08</v>
+      </c>
+      <c r="Z174" s="10">
+        <v>0.73428000000000004</v>
+      </c>
+      <c r="AA174" s="10">
+        <v>95</v>
+      </c>
+      <c r="AC174" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD174" s="10">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="P175" s="25"/>
+      <c r="R175" t="s">
+        <v>28</v>
+      </c>
+      <c r="S175" s="10">
+        <v>39</v>
+      </c>
+      <c r="T175" s="10">
+        <v>11</v>
+      </c>
+      <c r="U175" s="10">
+        <v>31</v>
+      </c>
+      <c r="V175" s="10">
+        <v>9</v>
+      </c>
+      <c r="W175" s="10">
+        <v>8</v>
+      </c>
+      <c r="X175" s="10">
+        <v>2</v>
+      </c>
+      <c r="Y175" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z175" s="10">
+        <v>1.4186300000000001</v>
+      </c>
+      <c r="AA175" s="10">
+        <v>91</v>
+      </c>
+      <c r="AC175" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD175" s="10">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="P176" s="25"/>
+      <c r="R176" t="s">
+        <v>29</v>
+      </c>
+      <c r="S176" s="10">
+        <v>25</v>
+      </c>
+      <c r="T176" s="10">
+        <v>20.83</v>
+      </c>
+      <c r="U176" s="10">
+        <v>23.96</v>
+      </c>
+      <c r="V176" s="10">
+        <v>12.5</v>
+      </c>
+      <c r="W176" s="10">
+        <v>11.46</v>
+      </c>
+      <c r="X176" s="10">
+        <v>4.17</v>
+      </c>
+      <c r="Y176" s="10">
+        <v>2.08</v>
+      </c>
+      <c r="Z176" s="10">
+        <v>0.27718999999999999</v>
+      </c>
+      <c r="AA176" s="10">
+        <v>100</v>
+      </c>
+      <c r="AC176" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD176" s="10">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="177" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P177" s="25"/>
+      <c r="R177" t="s">
+        <v>30</v>
+      </c>
+      <c r="S177" s="10">
+        <v>38</v>
+      </c>
+      <c r="T177" s="10">
+        <v>16</v>
+      </c>
+      <c r="U177" s="10">
+        <v>18</v>
+      </c>
+      <c r="V177" s="10">
+        <v>15</v>
+      </c>
+      <c r="W177" s="10">
+        <v>7</v>
+      </c>
+      <c r="X177" s="10">
+        <v>5</v>
+      </c>
+      <c r="Y177" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z177" s="10">
+        <v>1.39438</v>
+      </c>
+      <c r="AA177" s="10">
+        <v>95</v>
+      </c>
+      <c r="AC177" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD177" s="10">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="178" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P178" s="25"/>
+      <c r="R178" t="s">
+        <v>92</v>
+      </c>
+      <c r="S178" s="10">
+        <v>20.41</v>
+      </c>
+      <c r="T178" s="10">
+        <v>22.45</v>
+      </c>
+      <c r="U178" s="10">
+        <v>24.49</v>
+      </c>
+      <c r="V178" s="10">
+        <v>9.18</v>
+      </c>
+      <c r="W178" s="10">
+        <v>7.14</v>
+      </c>
+      <c r="X178" s="10">
+        <v>7.14</v>
+      </c>
+      <c r="Y178" s="10">
+        <v>9.18</v>
+      </c>
+      <c r="Z178" s="10">
+        <v>0.57791000000000003</v>
+      </c>
+      <c r="AA178" s="10">
+        <v>97</v>
+      </c>
+      <c r="AC178" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD178" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="179" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P179" s="25"/>
+      <c r="R179" t="s">
+        <v>93</v>
+      </c>
+      <c r="S179" s="10">
+        <v>36.36</v>
+      </c>
+      <c r="T179" s="10">
+        <v>12.12</v>
+      </c>
+      <c r="U179" s="10">
+        <v>19.190000000000001</v>
+      </c>
+      <c r="V179" s="10">
+        <v>18.18</v>
+      </c>
+      <c r="W179" s="10">
+        <v>8.08</v>
+      </c>
+      <c r="X179" s="10">
+        <v>5.05</v>
+      </c>
+      <c r="Y179" s="10">
+        <v>1.01</v>
+      </c>
+      <c r="Z179" s="10">
+        <v>1.52136</v>
+      </c>
+      <c r="AA179" s="10">
+        <v>97</v>
+      </c>
+      <c r="AC179" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD179" s="10">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="180" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P180" s="25"/>
+      <c r="R180" t="s">
+        <v>94</v>
+      </c>
+      <c r="S180" s="10">
+        <v>16.84</v>
+      </c>
+      <c r="T180" s="10">
+        <v>25.26</v>
+      </c>
+      <c r="U180" s="10">
+        <v>20</v>
+      </c>
+      <c r="V180" s="10">
+        <v>16.84</v>
+      </c>
+      <c r="W180" s="10">
+        <v>12.63</v>
+      </c>
+      <c r="X180" s="10">
+        <v>6.32</v>
+      </c>
+      <c r="Y180" s="10">
+        <v>2.11</v>
+      </c>
+      <c r="Z180" s="10">
+        <v>0.22189999999999999</v>
+      </c>
+      <c r="AA180" s="10">
+        <v>98</v>
+      </c>
+      <c r="AC180" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD180" s="10">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="181" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P181" s="25"/>
+      <c r="R181" t="s">
+        <v>95</v>
+      </c>
+      <c r="S181" s="10">
+        <v>44</v>
+      </c>
+      <c r="T181" s="10">
+        <v>9</v>
+      </c>
+      <c r="U181" s="10">
+        <v>31</v>
+      </c>
+      <c r="V181" s="10">
+        <v>10</v>
+      </c>
+      <c r="W181" s="10">
+        <v>5</v>
+      </c>
+      <c r="X181" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y181" s="10">
+        <v>1</v>
+      </c>
+      <c r="Z181" s="10">
+        <v>0.93274999999999997</v>
+      </c>
+      <c r="AA181" s="10">
+        <v>95</v>
+      </c>
+      <c r="AC181" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD181" s="10">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="182" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P182" s="25"/>
+      <c r="R182" t="s">
+        <v>71</v>
+      </c>
+      <c r="S182" s="10">
+        <v>29.17</v>
+      </c>
+      <c r="T182" s="10">
+        <v>26.04</v>
+      </c>
+      <c r="U182" s="10">
+        <v>19.79</v>
+      </c>
+      <c r="V182" s="10">
+        <v>11.46</v>
+      </c>
+      <c r="W182" s="10">
+        <v>8.33</v>
+      </c>
+      <c r="X182" s="10">
+        <v>1.04</v>
+      </c>
+      <c r="Y182" s="10">
+        <v>4.17</v>
+      </c>
+      <c r="Z182" s="10">
+        <v>0.99038999999999999</v>
+      </c>
+      <c r="AA182" s="10">
+        <v>94</v>
+      </c>
+      <c r="AC182" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD182" s="10">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="183" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P183" s="25"/>
+      <c r="R183" t="s">
+        <v>72</v>
+      </c>
+      <c r="S183" s="10">
+        <v>37</v>
+      </c>
+      <c r="T183" s="10">
+        <v>16</v>
+      </c>
+      <c r="U183" s="10">
+        <v>29</v>
+      </c>
+      <c r="V183" s="10">
+        <v>13</v>
+      </c>
+      <c r="W183" s="10">
+        <v>2</v>
+      </c>
+      <c r="X183" s="10">
+        <v>3</v>
+      </c>
+      <c r="Y183" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z183" s="10">
+        <v>1.478</v>
+      </c>
+      <c r="AA183" s="10">
+        <v>94</v>
+      </c>
+      <c r="AC183" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD183" s="10">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="184" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P184" s="25"/>
+      <c r="R184" t="s">
+        <v>73</v>
+      </c>
+      <c r="S184" s="10">
+        <v>25.77</v>
+      </c>
+      <c r="T184" s="10">
+        <v>21.65</v>
+      </c>
+      <c r="U184" s="10">
+        <v>20.62</v>
+      </c>
+      <c r="V184" s="10">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="W184" s="10">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="X184" s="10">
+        <v>2.06</v>
+      </c>
+      <c r="Y184" s="10">
+        <v>4.12</v>
+      </c>
+      <c r="Z184" s="10">
+        <v>0.18287</v>
+      </c>
+      <c r="AA184" s="10">
+        <v>98</v>
+      </c>
+      <c r="AC184" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD184" s="10">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="185" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P185" s="25"/>
+      <c r="R185" t="s">
+        <v>74</v>
+      </c>
+      <c r="S185" s="10">
+        <v>21.28</v>
+      </c>
+      <c r="T185" s="10">
+        <v>27.66</v>
+      </c>
+      <c r="U185" s="10">
+        <v>22.34</v>
+      </c>
+      <c r="V185" s="10">
+        <v>10.64</v>
+      </c>
+      <c r="W185" s="10">
+        <v>10.64</v>
+      </c>
+      <c r="X185" s="10">
+        <v>6.38</v>
+      </c>
+      <c r="Y185" s="10">
+        <v>1.06</v>
+      </c>
+      <c r="Z185" s="10">
+        <v>2.5708700000000002</v>
+      </c>
+      <c r="AA185" s="10">
+        <v>99</v>
+      </c>
+      <c r="AC185" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD185" s="10">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="186" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P186" s="25"/>
+      <c r="R186" t="s">
+        <v>75</v>
+      </c>
+      <c r="S186" s="10">
+        <v>25.51</v>
+      </c>
+      <c r="T186" s="10">
+        <v>25.51</v>
+      </c>
+      <c r="U186" s="10">
+        <v>26.53</v>
+      </c>
+      <c r="V186" s="10">
+        <v>4.08</v>
+      </c>
+      <c r="W186" s="10">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="X186" s="10">
+        <v>4.08</v>
+      </c>
+      <c r="Y186" s="10">
+        <v>4.08</v>
+      </c>
+      <c r="Z186" s="10">
+        <v>1.04128</v>
+      </c>
+      <c r="AA186" s="10">
+        <v>94</v>
+      </c>
+      <c r="AC186" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD186" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P187" s="25"/>
+      <c r="R187" t="s">
+        <v>76</v>
+      </c>
+      <c r="S187" s="10">
+        <v>48</v>
+      </c>
+      <c r="T187" s="10">
+        <v>12</v>
+      </c>
+      <c r="U187" s="10">
+        <v>26</v>
+      </c>
+      <c r="V187" s="10">
+        <v>10</v>
+      </c>
+      <c r="W187" s="10">
+        <v>2</v>
+      </c>
+      <c r="X187" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y187" s="10">
+        <v>2</v>
+      </c>
+      <c r="Z187" s="10">
+        <v>1.26867</v>
+      </c>
+      <c r="AA187" s="10">
+        <v>97</v>
+      </c>
+      <c r="AC187" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD187" s="10">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="188" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P188" s="25"/>
+      <c r="R188" t="s">
+        <v>77</v>
+      </c>
+      <c r="S188" s="10">
+        <v>25.25</v>
+      </c>
+      <c r="T188" s="10">
+        <v>23.23</v>
+      </c>
+      <c r="U188" s="10">
+        <v>15.15</v>
+      </c>
+      <c r="V188" s="10">
+        <v>16.16</v>
+      </c>
+      <c r="W188" s="10">
+        <v>9.09</v>
+      </c>
+      <c r="X188" s="10">
+        <v>7.07</v>
+      </c>
+      <c r="Y188" s="10">
+        <v>4.04</v>
+      </c>
+      <c r="Z188" s="10">
+        <v>0.25139</v>
+      </c>
+      <c r="AA188" s="10">
+        <v>99</v>
+      </c>
+      <c r="AC188" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD188" s="10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="189" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P189" s="25"/>
+      <c r="R189" t="s">
+        <v>78</v>
+      </c>
+      <c r="S189" s="10">
+        <v>32.99</v>
+      </c>
+      <c r="T189" s="10">
+        <v>15.46</v>
+      </c>
+      <c r="U189" s="10">
+        <v>31.96</v>
+      </c>
+      <c r="V189" s="10">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="W189" s="10">
+        <v>4.12</v>
+      </c>
+      <c r="X189" s="10">
+        <v>3.09</v>
+      </c>
+      <c r="Y189" s="10">
+        <v>3.09</v>
+      </c>
+      <c r="Z189" s="10">
+        <v>12.11806</v>
+      </c>
+      <c r="AA189" s="10">
+        <v>98</v>
+      </c>
+      <c r="AC189" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD189" s="10">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="190" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P190" s="25"/>
+      <c r="AD190" s="14"/>
+    </row>
+    <row r="191" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P191" s="25"/>
+      <c r="R191" t="s">
+        <v>39</v>
+      </c>
+      <c r="S191" s="10">
+        <v>26.53</v>
+      </c>
+      <c r="T191" s="10">
+        <v>21.43</v>
+      </c>
+      <c r="U191" s="10">
+        <v>18.37</v>
+      </c>
+      <c r="V191" s="10">
+        <v>12.24</v>
+      </c>
+      <c r="W191" s="10">
+        <v>9.18</v>
+      </c>
+      <c r="X191" s="10">
+        <v>9.18</v>
+      </c>
+      <c r="Y191" s="10">
+        <v>3.06</v>
+      </c>
+      <c r="Z191" s="10">
+        <v>2.6934499999999999</v>
+      </c>
+      <c r="AA191" s="10">
+        <v>96</v>
+      </c>
+      <c r="AC191" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD191" s="10">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="192" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P192" s="25"/>
+      <c r="R192" t="s">
+        <v>40</v>
+      </c>
+      <c r="S192" s="10">
+        <v>24.74</v>
+      </c>
+      <c r="T192" s="10">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="U192" s="10">
+        <v>20.62</v>
+      </c>
+      <c r="V192" s="10">
+        <v>14.43</v>
+      </c>
+      <c r="W192" s="10">
+        <v>8.25</v>
+      </c>
+      <c r="X192" s="10">
+        <v>7.22</v>
+      </c>
+      <c r="Y192" s="10">
+        <v>6.19</v>
+      </c>
+      <c r="Z192" s="10">
+        <v>0.65271000000000001</v>
+      </c>
+      <c r="AA192" s="10">
+        <v>96</v>
+      </c>
+      <c r="AC192" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD192" s="10">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="193" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P193" s="25"/>
+      <c r="R193" t="s">
+        <v>41</v>
+      </c>
+      <c r="S193" s="10">
+        <v>23.47</v>
+      </c>
+      <c r="T193" s="10">
+        <v>20.41</v>
+      </c>
+      <c r="U193" s="10">
+        <v>19.39</v>
+      </c>
+      <c r="V193" s="10">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="W193" s="10">
+        <v>15.31</v>
+      </c>
+      <c r="X193" s="10">
+        <v>1.02</v>
+      </c>
+      <c r="Y193" s="10">
+        <v>4.08</v>
+      </c>
+      <c r="Z193" s="10">
+        <v>2.7113900000000002</v>
+      </c>
+      <c r="AA193" s="10">
+        <v>97</v>
+      </c>
+      <c r="AC193" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD193" s="10">
+        <v>11.6</v>
+      </c>
+    </row>
+    <row r="194" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P194" s="25"/>
+      <c r="R194" t="s">
+        <v>42</v>
+      </c>
+      <c r="S194" s="10">
+        <v>25.53</v>
+      </c>
+      <c r="T194" s="10">
+        <v>15.96</v>
+      </c>
+      <c r="U194" s="10">
+        <v>23.4</v>
+      </c>
+      <c r="V194" s="10">
+        <v>13.83</v>
+      </c>
+      <c r="W194" s="10">
+        <v>11.7</v>
+      </c>
+      <c r="X194" s="10">
+        <v>7.45</v>
+      </c>
+      <c r="Y194" s="10">
+        <v>2.13</v>
+      </c>
+      <c r="Z194" s="10">
+        <v>0.40225</v>
+      </c>
+      <c r="AA194" s="10">
+        <v>97</v>
+      </c>
+      <c r="AC194" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD194" s="10">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="195" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P195" s="25"/>
+      <c r="R195" t="s">
+        <v>43</v>
+      </c>
+      <c r="S195" s="10">
+        <v>31.52</v>
+      </c>
+      <c r="T195" s="10">
+        <v>21.74</v>
+      </c>
+      <c r="U195" s="10">
+        <v>15.22</v>
+      </c>
+      <c r="V195" s="10">
+        <v>11.96</v>
+      </c>
+      <c r="W195" s="10">
+        <v>11.96</v>
+      </c>
+      <c r="X195" s="10">
+        <v>5.43</v>
+      </c>
+      <c r="Y195" s="10">
+        <v>2.17</v>
+      </c>
+      <c r="Z195" s="10">
+        <v>1.93943</v>
+      </c>
+      <c r="AA195" s="10">
+        <v>90</v>
+      </c>
+      <c r="AC195" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD195" s="10">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="196" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P196" s="25"/>
+      <c r="R196" t="s">
+        <v>44</v>
+      </c>
+      <c r="S196" s="10">
+        <v>25.26</v>
+      </c>
+      <c r="T196" s="10">
+        <v>18.95</v>
+      </c>
+      <c r="U196" s="10">
+        <v>23.16</v>
+      </c>
+      <c r="V196" s="10">
+        <v>10.53</v>
+      </c>
+      <c r="W196" s="10">
+        <v>11.58</v>
+      </c>
+      <c r="X196" s="10">
+        <v>7.37</v>
+      </c>
+      <c r="Y196" s="10">
+        <v>3.16</v>
+      </c>
+      <c r="Z196" s="10">
+        <v>0.40512999999999999</v>
+      </c>
+      <c r="AA196" s="10">
+        <v>97</v>
+      </c>
+      <c r="AC196" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD196" s="10">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="197" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P197" s="25"/>
+      <c r="R197" t="s">
+        <v>45</v>
+      </c>
+      <c r="S197" s="10">
+        <v>20.62</v>
+      </c>
+      <c r="T197" s="10">
+        <v>19.59</v>
+      </c>
+      <c r="U197" s="10">
+        <v>18.559999999999999</v>
+      </c>
+      <c r="V197" s="10">
+        <v>15.46</v>
+      </c>
+      <c r="W197" s="10">
+        <v>13.4</v>
+      </c>
+      <c r="X197" s="10">
+        <v>8.25</v>
+      </c>
+      <c r="Y197" s="10">
+        <v>4.12</v>
+      </c>
+      <c r="Z197" s="10">
+        <v>2.22282</v>
+      </c>
+      <c r="AA197" s="10">
+        <v>97</v>
+      </c>
+      <c r="AC197" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD197" s="10">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="198" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P198" s="25"/>
+      <c r="R198" t="s">
+        <v>46</v>
+      </c>
+      <c r="S198" s="10">
+        <v>25.81</v>
+      </c>
+      <c r="T198" s="10">
+        <v>15.05</v>
+      </c>
+      <c r="U198" s="10">
+        <v>21.51</v>
+      </c>
+      <c r="V198" s="10">
+        <v>17.2</v>
+      </c>
+      <c r="W198" s="10">
+        <v>8.6</v>
+      </c>
+      <c r="X198" s="10">
+        <v>4.3</v>
+      </c>
+      <c r="Y198" s="10">
+        <v>7.53</v>
+      </c>
+      <c r="Z198" s="10">
+        <v>0.47400999999999999</v>
+      </c>
+      <c r="AA198" s="10">
+        <v>95</v>
+      </c>
+      <c r="AC198" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD198" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="199" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P199" s="25"/>
+      <c r="R199" t="s">
+        <v>47</v>
+      </c>
+      <c r="S199" s="10">
+        <v>26.8</v>
+      </c>
+      <c r="T199" s="10">
+        <v>24.74</v>
+      </c>
+      <c r="U199" s="10">
+        <v>17.53</v>
+      </c>
+      <c r="V199" s="10">
+        <v>11.34</v>
+      </c>
+      <c r="W199" s="10">
+        <v>12.37</v>
+      </c>
+      <c r="X199" s="10">
+        <v>4.12</v>
+      </c>
+      <c r="Y199" s="10">
+        <v>3.09</v>
+      </c>
+      <c r="Z199" s="10">
+        <v>2.2191999999999998</v>
+      </c>
+      <c r="AA199" s="10">
+        <v>95</v>
+      </c>
+      <c r="AC199" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD199" s="10">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="200" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P200" s="25"/>
+      <c r="R200" t="s">
+        <v>48</v>
+      </c>
+      <c r="S200" s="10">
+        <v>25.81</v>
+      </c>
+      <c r="T200" s="10">
+        <v>15.05</v>
+      </c>
+      <c r="U200" s="10">
+        <v>21.51</v>
+      </c>
+      <c r="V200" s="10">
+        <v>17.2</v>
+      </c>
+      <c r="W200" s="10">
+        <v>8.6</v>
+      </c>
+      <c r="X200" s="10">
+        <v>4.3</v>
+      </c>
+      <c r="Y200" s="10">
+        <v>7.53</v>
+      </c>
+      <c r="Z200" s="10">
+        <v>0.47395999999999999</v>
+      </c>
+      <c r="AA200" s="10">
+        <v>95</v>
+      </c>
+      <c r="AC200" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD200" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="201" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P201" s="25"/>
+      <c r="R201" t="s">
+        <v>96</v>
+      </c>
+      <c r="S201" s="10">
+        <v>23.16</v>
+      </c>
+      <c r="T201" s="10">
+        <v>20</v>
+      </c>
+      <c r="U201" s="10">
+        <v>18.95</v>
+      </c>
+      <c r="V201" s="10">
+        <v>14.74</v>
+      </c>
+      <c r="W201" s="10">
+        <v>15.79</v>
+      </c>
+      <c r="X201" s="10">
+        <v>6.32</v>
+      </c>
+      <c r="Y201" s="10">
+        <v>1.05</v>
+      </c>
+      <c r="Z201" s="10">
+        <v>2.2895699999999999</v>
+      </c>
+      <c r="AA201" s="10">
+        <v>92</v>
+      </c>
+      <c r="AC201" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD201" s="10">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="202" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P202" s="25"/>
+      <c r="R202" t="s">
+        <v>97</v>
+      </c>
+      <c r="S202" s="10">
+        <v>31.11</v>
+      </c>
+      <c r="T202" s="10">
+        <v>18.89</v>
+      </c>
+      <c r="U202" s="10">
+        <v>14.44</v>
+      </c>
+      <c r="V202" s="10">
+        <v>12.22</v>
+      </c>
+      <c r="W202" s="10">
+        <v>15.56</v>
+      </c>
+      <c r="X202" s="10">
+        <v>6.67</v>
+      </c>
+      <c r="Y202" s="10">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="Z202" s="10">
+        <v>0.61975000000000002</v>
+      </c>
+      <c r="AA202" s="10">
+        <v>97</v>
+      </c>
+      <c r="AC202" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD202" s="10">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="203" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P203" s="25"/>
+      <c r="R203" t="s">
+        <v>81</v>
+      </c>
+      <c r="S203" s="10">
+        <v>23.47</v>
+      </c>
+      <c r="T203" s="10">
+        <v>19.39</v>
+      </c>
+      <c r="U203" s="10">
+        <v>19.39</v>
+      </c>
+      <c r="V203" s="10">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="W203" s="10">
+        <v>14.29</v>
+      </c>
+      <c r="X203" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Y203" s="10">
+        <v>2.04</v>
+      </c>
+      <c r="Z203" s="10">
+        <v>2.2624200000000001</v>
+      </c>
+      <c r="AA203" s="10">
+        <v>96</v>
+      </c>
+      <c r="AC203" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD203" s="10">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="204" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P204" s="25"/>
+      <c r="R204" t="s">
+        <v>82</v>
+      </c>
+      <c r="S204" s="10">
+        <v>21.88</v>
+      </c>
+      <c r="T204" s="10">
+        <v>14.58</v>
+      </c>
+      <c r="U204" s="10">
+        <v>23.96</v>
+      </c>
+      <c r="V204" s="10">
+        <v>19.79</v>
+      </c>
+      <c r="W204" s="10">
+        <v>8.33</v>
+      </c>
+      <c r="X204" s="10">
+        <v>6.25</v>
+      </c>
+      <c r="Y204" s="10">
+        <v>5.21</v>
+      </c>
+      <c r="Z204" s="10">
+        <v>0.47821999999999998</v>
+      </c>
+      <c r="AA204" s="10">
+        <v>98</v>
+      </c>
+      <c r="AC204" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD204" s="10">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="205" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P205" s="25"/>
+      <c r="R205" t="s">
+        <v>83</v>
+      </c>
+      <c r="S205" s="10">
+        <v>26.32</v>
+      </c>
+      <c r="T205" s="10">
+        <v>20</v>
+      </c>
+      <c r="U205" s="10">
+        <v>16.84</v>
+      </c>
+      <c r="V205" s="10">
+        <v>12.63</v>
+      </c>
+      <c r="W205" s="10">
+        <v>13.68</v>
+      </c>
+      <c r="X205" s="10">
+        <v>6.32</v>
+      </c>
+      <c r="Y205" s="10">
+        <v>4.21</v>
+      </c>
+      <c r="Z205" s="10">
+        <v>1.9125099999999999</v>
+      </c>
+      <c r="AA205" s="10">
+        <v>94</v>
+      </c>
+      <c r="AC205" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD205" s="10">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="206" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P206" s="25"/>
+      <c r="R206" t="s">
+        <v>84</v>
+      </c>
+      <c r="S206" s="10">
+        <v>33.67</v>
+      </c>
+      <c r="T206" s="10">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="U206" s="10">
+        <v>22.45</v>
+      </c>
+      <c r="V206" s="10">
+        <v>15.31</v>
+      </c>
+      <c r="W206" s="10">
+        <v>6.12</v>
+      </c>
+      <c r="X206" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Y206" s="10">
+        <v>1.02</v>
+      </c>
+      <c r="Z206" s="10">
+        <v>9.6793800000000001</v>
+      </c>
+      <c r="AA206" s="10">
+        <v>99</v>
+      </c>
+      <c r="AC206" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD206" s="10">
+        <v>43.2</v>
+      </c>
+    </row>
+    <row r="207" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P207" s="25"/>
+    </row>
+    <row r="208" spans="16:30" x14ac:dyDescent="0.35">
+      <c r="P208" s="25"/>
+      <c r="R208" t="s">
+        <v>49</v>
+      </c>
+      <c r="S208" s="10">
+        <f t="shared" ref="S208:Y208" si="24">AVERAGE(S158:S189,S191:S206)</f>
+        <v>28.627291666666661</v>
+      </c>
+      <c r="T208" s="10">
+        <f t="shared" si="24"/>
+        <v>18.235000000000003</v>
+      </c>
+      <c r="U208" s="10">
+        <f t="shared" si="24"/>
+        <v>21.556666666666668</v>
+      </c>
+      <c r="V208" s="10">
+        <f t="shared" si="24"/>
+        <v>13.719999999999999</v>
+      </c>
+      <c r="W208" s="10">
+        <f t="shared" si="24"/>
+        <v>9.5012500000000006</v>
+      </c>
+      <c r="X208" s="10">
+        <f t="shared" si="24"/>
+        <v>5.206666666666667</v>
+      </c>
+      <c r="Y208" s="10">
+        <f t="shared" si="24"/>
+        <v>3.1516666666666677</v>
+      </c>
+      <c r="Z208" s="1"/>
+      <c r="AA208" s="14">
+        <f>SUM(AA158:AA206)</f>
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="209" spans="16:28" x14ac:dyDescent="0.35">
+      <c r="P209" s="25"/>
+    </row>
+    <row r="210" spans="16:28" x14ac:dyDescent="0.35">
+      <c r="P210" s="25"/>
+      <c r="R210" t="s">
+        <v>52</v>
+      </c>
+      <c r="V210" s="14"/>
+      <c r="W210" s="19"/>
+      <c r="X210" s="19"/>
+      <c r="Z210" s="14">
+        <f>AVERAGE(Z158:Z189)</f>
+        <v>1.4379021875</v>
+      </c>
+      <c r="AA210" s="14"/>
+    </row>
+    <row r="211" spans="16:28" x14ac:dyDescent="0.35">
+      <c r="P211" s="25"/>
+      <c r="R211" t="s">
+        <v>53</v>
+      </c>
+      <c r="W211" s="19"/>
+      <c r="X211" s="19"/>
+      <c r="Z211" s="14">
+        <f>AVERAGE(Z191:Z206)</f>
+        <v>1.9647625</v>
+      </c>
+      <c r="AA211" s="14"/>
+    </row>
+    <row r="212" spans="16:28" x14ac:dyDescent="0.35">
+      <c r="P212" s="25"/>
+      <c r="W212" s="19"/>
+      <c r="X212" s="19"/>
+      <c r="AA212" s="14"/>
+    </row>
+    <row r="213" spans="16:28" x14ac:dyDescent="0.35">
+      <c r="P213" s="25"/>
+      <c r="R213" t="s">
+        <v>57</v>
+      </c>
+      <c r="W213" s="19"/>
+      <c r="X213" s="19"/>
+      <c r="AA213" s="24">
+        <f>SUM(AA158:AA206) / (48*100)</f>
+        <v>0.95770833333333338</v>
+      </c>
+      <c r="AB213" s="14"/>
+    </row>
+    <row r="214" spans="16:28" x14ac:dyDescent="0.35">
+      <c r="P214" s="25"/>
+    </row>
+    <row r="215" spans="16:28" x14ac:dyDescent="0.35">
+      <c r="P215" s="25"/>
+    </row>
+    <row r="216" spans="16:28" x14ac:dyDescent="0.35">
+      <c r="P216" s="25"/>
+    </row>
+    <row r="217" spans="16:28" x14ac:dyDescent="0.35">
+      <c r="P217" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>